<commit_message>
Improved Node Appearance Rate.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/TOSobserved.xlsx
+++ b/Prototypes/Mungbean/TOSobserved.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47416035-770D-4E85-9F87-FD5B58D40027}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C397C1F-FC9E-4AFD-989A-E8DDF6929C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="345" windowWidth="10785" windowHeight="10800" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$AD$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$AE$151</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="78">
   <si>
     <t>Location</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>Vegetative</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.BranchNumber</t>
   </si>
 </sst>
 </file>
@@ -689,11 +692,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3519DD51-BED6-4262-8A50-4DB48CCAF26B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AE151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG128" sqref="AG128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -791,14 +795,16 @@
         <v>11</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3"/>
-    </row>
-    <row r="2" spans="1:31">
+      <c r="AE1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" hidden="1">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -860,7 +866,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" hidden="1">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -943,7 +949,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" hidden="1">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" hidden="1">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" hidden="1">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1144,7 +1150,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" hidden="1">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" hidden="1">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1287,7 +1293,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" hidden="1">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1371,7 +1377,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" hidden="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1433,7 +1439,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" hidden="1">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" hidden="1">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1579,7 +1585,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" hidden="1">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" hidden="1">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1724,8 +1730,12 @@
       <c r="AD14">
         <v>0.41457809879442498</v>
       </c>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="AE14">
+        <f>AC14-1</f>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" hidden="1">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1786,8 +1796,12 @@
       <c r="AD15">
         <v>0.52796780204857408</v>
       </c>
-    </row>
-    <row r="16" spans="1:31">
+      <c r="AE15">
+        <f>AC15-1</f>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" hidden="1">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1870,8 +1884,12 @@
       <c r="AD16">
         <v>0.71239034243875055</v>
       </c>
-    </row>
-    <row r="17" spans="1:31">
+      <c r="AE16">
+        <f t="shared" ref="AE16:AE38" si="0">AC16-1</f>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" hidden="1">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1938,8 +1956,12 @@
       <c r="AD17">
         <v>0.44370598373247128</v>
       </c>
-    </row>
-    <row r="18" spans="1:31" s="9" customFormat="1">
+      <c r="AE17">
+        <f t="shared" si="0"/>
+        <v>11.049999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" s="9" customFormat="1" hidden="1">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2010,9 +2032,12 @@
       <c r="AD18">
         <v>0.58040933831219732</v>
       </c>
-      <c r="AE18"/>
-    </row>
-    <row r="19" spans="1:31" s="9" customFormat="1">
+      <c r="AE18">
+        <f t="shared" si="0"/>
+        <v>5.7499999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" s="9" customFormat="1" hidden="1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2083,9 +2108,12 @@
       <c r="AD19">
         <v>0.34910600109422335</v>
       </c>
-      <c r="AE19"/>
-    </row>
-    <row r="20" spans="1:31" s="9" customFormat="1">
+      <c r="AE19">
+        <f t="shared" si="0"/>
+        <v>7.0500000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" s="9" customFormat="1" hidden="1">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2171,9 +2199,12 @@
       <c r="AD20">
         <v>0.24874685927665507</v>
       </c>
-      <c r="AE20"/>
-    </row>
-    <row r="21" spans="1:31" s="9" customFormat="1">
+      <c r="AE20">
+        <f t="shared" si="0"/>
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" s="9" customFormat="1" hidden="1">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2248,9 +2279,12 @@
       <c r="AD21">
         <v>0.50249378105604425</v>
       </c>
-      <c r="AE21"/>
-    </row>
-    <row r="22" spans="1:31">
+      <c r="AE21">
+        <f t="shared" si="0"/>
+        <v>10.100000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" hidden="1">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2311,8 +2345,12 @@
       <c r="AD22">
         <v>0.36996621467371954</v>
       </c>
-    </row>
-    <row r="23" spans="1:31">
+      <c r="AE22">
+        <f t="shared" si="0"/>
+        <v>3.4499999999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" hidden="1">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2373,8 +2411,12 @@
       <c r="AD23">
         <v>0.43229041164476467</v>
       </c>
-    </row>
-    <row r="24" spans="1:31">
+      <c r="AE23">
+        <f t="shared" si="0"/>
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" hidden="1">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2441,8 +2483,12 @@
       <c r="AD24">
         <v>0.63786754110865884</v>
       </c>
-    </row>
-    <row r="25" spans="1:31">
+      <c r="AE24">
+        <f t="shared" si="0"/>
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" hidden="1">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2525,8 +2571,12 @@
       <c r="AD25">
         <v>0.50682837331783215</v>
       </c>
-    </row>
-    <row r="26" spans="1:31">
+      <c r="AE25">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" hidden="1">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2587,8 +2637,12 @@
       <c r="AD26">
         <v>0.5678908345800272</v>
       </c>
-    </row>
-    <row r="27" spans="1:31">
+      <c r="AE26">
+        <f t="shared" si="0"/>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" hidden="1">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -2649,8 +2703,12 @@
       <c r="AD27">
         <v>0.56734028589551277</v>
       </c>
-    </row>
-    <row r="28" spans="1:31">
+      <c r="AE27">
+        <f t="shared" si="0"/>
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" hidden="1">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -2733,8 +2791,12 @@
       <c r="AD28">
         <v>0.47696960070847289</v>
       </c>
-    </row>
-    <row r="29" spans="1:31">
+      <c r="AE28">
+        <f t="shared" si="0"/>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" hidden="1">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2801,8 +2863,12 @@
       <c r="AD29">
         <v>8.2915619758885034E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:31">
+      <c r="AE29">
+        <f t="shared" si="0"/>
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" hidden="1">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -2863,9 +2929,12 @@
       <c r="AD30">
         <v>0.73484692283495401</v>
       </c>
-      <c r="AE30" s="9"/>
-    </row>
-    <row r="31" spans="1:31">
+      <c r="AE30">
+        <f t="shared" si="0"/>
+        <v>5.1999999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" hidden="1">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2932,9 +3001,12 @@
       <c r="AD31">
         <v>0.55396299515400349</v>
       </c>
-      <c r="AE31" s="9"/>
-    </row>
-    <row r="32" spans="1:31">
+      <c r="AE31">
+        <f t="shared" si="0"/>
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" hidden="1">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2995,9 +3067,12 @@
       <c r="AD32">
         <v>0.70887234393788967</v>
       </c>
-      <c r="AE32" s="9"/>
-    </row>
-    <row r="33" spans="1:31">
+      <c r="AE32">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" hidden="1">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -3080,9 +3155,12 @@
       <c r="AD33">
         <v>0.44370598373247128</v>
       </c>
-      <c r="AE33" s="9"/>
-    </row>
-    <row r="34" spans="1:31">
+      <c r="AE33">
+        <f t="shared" si="0"/>
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" hidden="1">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3141,8 +3219,12 @@
       <c r="AD34">
         <v>0.37666297933298493</v>
       </c>
-    </row>
-    <row r="35" spans="1:31">
+      <c r="AE34">
+        <f t="shared" si="0"/>
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" hidden="1">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -3213,8 +3295,12 @@
       <c r="AD35">
         <v>0.60207972893961537</v>
       </c>
-    </row>
-    <row r="36" spans="1:31">
+      <c r="AE35">
+        <f t="shared" si="0"/>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" hidden="1">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -3277,8 +3363,12 @@
       <c r="AD36">
         <v>0.49180788932265013</v>
       </c>
-    </row>
-    <row r="37" spans="1:31">
+      <c r="AE36">
+        <f t="shared" si="0"/>
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" hidden="1">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -3364,8 +3454,12 @@
       <c r="AD37">
         <v>0.62849025449882356</v>
       </c>
-    </row>
-    <row r="38" spans="1:31">
+      <c r="AE37">
+        <f t="shared" si="0"/>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" hidden="1">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -3432,8 +3526,12 @@
       <c r="AD38">
         <v>1.1757976016304847</v>
       </c>
-    </row>
-    <row r="39" spans="1:31">
+      <c r="AE38">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" hidden="1">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -3489,7 +3587,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" hidden="1">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -3551,7 +3649,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" hidden="1">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -3629,7 +3727,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" hidden="1">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -3690,8 +3788,12 @@
       <c r="AD42">
         <v>8.2915619758885076E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:31">
+      <c r="AE42">
+        <f>AC42-1</f>
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" hidden="1">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -3758,8 +3860,12 @@
       <c r="AD43">
         <v>0.43301270189222135</v>
       </c>
-    </row>
-    <row r="44" spans="1:31">
+      <c r="AE43">
+        <f>AC43-1</f>
+        <v>6.8999999999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" hidden="1">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -3842,8 +3948,12 @@
       <c r="AD44">
         <v>0.23284920012746457</v>
       </c>
-    </row>
-    <row r="45" spans="1:31">
+      <c r="AE44">
+        <f t="shared" ref="AE44:AE51" si="1">AC44-1</f>
+        <v>10.875</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" hidden="1">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -3910,8 +4020,12 @@
       <c r="AD45">
         <v>0.49180788932264974</v>
       </c>
-    </row>
-    <row r="46" spans="1:31">
+      <c r="AE45">
+        <f t="shared" si="1"/>
+        <v>13.85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" hidden="1">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -3972,8 +4086,12 @@
       <c r="AD46">
         <v>0.47087020504593402</v>
       </c>
-    </row>
-    <row r="47" spans="1:31">
+      <c r="AE46">
+        <f t="shared" si="1"/>
+        <v>4.2750000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" hidden="1">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -4040,8 +4158,12 @@
       <c r="AD47">
         <v>0.68920243760451216</v>
       </c>
-    </row>
-    <row r="48" spans="1:31">
+      <c r="AE47">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" hidden="1">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -4124,8 +4246,12 @@
       <c r="AD48">
         <v>0.22484562605386729</v>
       </c>
-    </row>
-    <row r="49" spans="1:30">
+      <c r="AE48">
+        <f t="shared" si="1"/>
+        <v>10.433333333333332</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" hidden="1">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -4192,8 +4318,12 @@
       <c r="AD49">
         <v>1.3141061600951396</v>
       </c>
-    </row>
-    <row r="50" spans="1:30">
+      <c r="AE49">
+        <f t="shared" si="1"/>
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" hidden="1">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -4254,8 +4384,12 @@
       <c r="AD50">
         <v>0.27726341266023546</v>
       </c>
-    </row>
-    <row r="51" spans="1:30">
+      <c r="AE50">
+        <f t="shared" si="1"/>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" hidden="1">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -4322,8 +4456,12 @@
       <c r="AD51">
         <v>1.1884864324004689</v>
       </c>
-    </row>
-    <row r="52" spans="1:30">
+      <c r="AE51">
+        <f t="shared" si="1"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" hidden="1">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -4385,7 +4523,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:31" hidden="1">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -4463,7 +4601,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:30">
+    <row r="54" spans="1:31" hidden="1">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -4530,8 +4668,12 @@
       <c r="AD54">
         <v>0.1732050807568877</v>
       </c>
-    </row>
-    <row r="55" spans="1:30">
+      <c r="AE54">
+        <f>AC54-1</f>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" hidden="1">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -4614,8 +4756,12 @@
       <c r="AD55">
         <v>0.81499616563515842</v>
       </c>
-    </row>
-    <row r="56" spans="1:30">
+      <c r="AE55">
+        <f>AC55-1</f>
+        <v>11.475</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" hidden="1">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -4682,8 +4828,12 @@
       <c r="AD56">
         <v>0.28145825622994264</v>
       </c>
-    </row>
-    <row r="57" spans="1:30">
+      <c r="AE56">
+        <f t="shared" ref="AE56" si="2">AC56-1</f>
+        <v>12.525</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" hidden="1">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -4739,7 +4889,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:31" hidden="1">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -4800,8 +4950,12 @@
       <c r="AD58">
         <v>0.43229041164476623</v>
       </c>
-    </row>
-    <row r="59" spans="1:30">
+      <c r="AE58">
+        <f>AC58-1</f>
+        <v>4.4499999999999993</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" hidden="1">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -4868,8 +5022,12 @@
       <c r="AD59">
         <v>1.0353139620424348</v>
       </c>
-    </row>
-    <row r="60" spans="1:30">
+      <c r="AE59">
+        <f>AC59-1</f>
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" hidden="1">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -4952,8 +5110,12 @@
       <c r="AD60">
         <v>0.33541019662496857</v>
       </c>
-    </row>
-    <row r="61" spans="1:30">
+      <c r="AE60">
+        <f t="shared" ref="AE60:AE63" si="3">AC60-1</f>
+        <v>10.899999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" hidden="1">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -5020,8 +5182,12 @@
       <c r="AD61">
         <v>1.3827056809024814</v>
       </c>
-    </row>
-    <row r="62" spans="1:30">
+      <c r="AE61">
+        <f t="shared" si="3"/>
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" hidden="1">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -5088,8 +5254,12 @@
       <c r="AD62">
         <v>0.68590724591594887</v>
       </c>
-    </row>
-    <row r="63" spans="1:30">
+      <c r="AE62">
+        <f t="shared" si="3"/>
+        <v>7.1749999999999989</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" hidden="1">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -5156,8 +5326,12 @@
       <c r="AD63">
         <v>1.7846568297574714</v>
       </c>
-    </row>
-    <row r="64" spans="1:30">
+      <c r="AE63">
+        <f t="shared" si="3"/>
+        <v>12.400000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" hidden="1">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -5213,7 +5387,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:31" hidden="1">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -5291,7 +5465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:30">
+    <row r="66" spans="1:31" hidden="1">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -5358,8 +5532,12 @@
       <c r="AD66">
         <v>0.18708286933869706</v>
       </c>
-    </row>
-    <row r="67" spans="1:30">
+      <c r="AE66">
+        <f>AC66-1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31" hidden="1">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -5442,8 +5620,12 @@
       <c r="AD67">
         <v>0.26809513236909011</v>
       </c>
-    </row>
-    <row r="68" spans="1:30">
+      <c r="AE67">
+        <f>AC67-1</f>
+        <v>7.3500000000000014</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31" hidden="1">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -5499,7 +5681,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:30">
+    <row r="69" spans="1:31" hidden="1">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -5561,7 +5743,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:30">
+    <row r="70" spans="1:31" hidden="1">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -5622,8 +5804,12 @@
       <c r="AD70">
         <v>0.55452682532047171</v>
       </c>
-    </row>
-    <row r="71" spans="1:30">
+      <c r="AE70">
+        <f>AC70-1</f>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31" hidden="1">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -5706,8 +5892,12 @@
       <c r="AD71">
         <v>0.71763500472036656</v>
       </c>
-    </row>
-    <row r="72" spans="1:30">
+      <c r="AE71">
+        <f>AC71-1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31" hidden="1">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -5774,8 +5964,12 @@
       <c r="AD72">
         <v>0.7595228765481663</v>
       </c>
-    </row>
-    <row r="73" spans="1:30">
+      <c r="AE72">
+        <f>AC72-1</f>
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31" hidden="1">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -5831,7 +6025,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:30">
+    <row r="74" spans="1:31" hidden="1">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -5898,8 +6092,12 @@
       <c r="AD74">
         <v>0.59319052588523336</v>
       </c>
-    </row>
-    <row r="75" spans="1:30">
+      <c r="AE74">
+        <f>AC74-1</f>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" hidden="1">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -5966,8 +6164,12 @@
       <c r="AD75">
         <v>0.81192287195274837</v>
       </c>
-    </row>
-    <row r="76" spans="1:30">
+      <c r="AE75">
+        <f>AC75-1</f>
+        <v>5.3250000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31" hidden="1">
       <c r="A76" t="s">
         <v>18</v>
       </c>
@@ -6023,7 +6225,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:30">
+    <row r="77" spans="1:31" hidden="1">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -6101,7 +6303,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:30">
+    <row r="78" spans="1:31" hidden="1">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -6168,8 +6370,12 @@
       <c r="AD78">
         <v>0.43011626335213293</v>
       </c>
-    </row>
-    <row r="79" spans="1:30">
+      <c r="AE78">
+        <f>AC78-1</f>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:31" hidden="1">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -6252,8 +6458,12 @@
       <c r="AD79">
         <v>0.11388041973930381</v>
       </c>
-    </row>
-    <row r="80" spans="1:30">
+      <c r="AE79">
+        <f>AC79-1</f>
+        <v>5.0250000000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31" hidden="1">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -6309,7 +6519,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:31" hidden="1">
       <c r="A81" t="s">
         <v>18</v>
       </c>
@@ -6371,7 +6581,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:31" hidden="1">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -6432,8 +6642,12 @@
       <c r="AD82">
         <v>0.31917863337009217</v>
       </c>
-    </row>
-    <row r="83" spans="1:30">
+      <c r="AE82">
+        <f>AC82-1</f>
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:31" hidden="1">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -6516,8 +6730,12 @@
       <c r="AD83">
         <v>0.24874685927665491</v>
       </c>
-    </row>
-    <row r="84" spans="1:30">
+      <c r="AE83">
+        <f>AC83-1</f>
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:31" hidden="1">
       <c r="A84" t="s">
         <v>18</v>
       </c>
@@ -6584,8 +6802,12 @@
       <c r="AD84">
         <v>0.58309518948452843</v>
       </c>
-    </row>
-    <row r="85" spans="1:30">
+      <c r="AE84">
+        <f>AC84-1</f>
+        <v>6.8000000000000007</v>
+      </c>
+    </row>
+    <row r="85" spans="1:31" hidden="1">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -6641,7 +6863,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:31">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -6662,8 +6884,12 @@
       <c r="AD86">
         <v>0.10897247358851676</v>
       </c>
-    </row>
-    <row r="87" spans="1:30">
+      <c r="AE86">
+        <f>AC86-1</f>
+        <v>4.5500000000000007</v>
+      </c>
+    </row>
+    <row r="87" spans="1:31">
       <c r="A87" t="s">
         <v>18</v>
       </c>
@@ -6700,8 +6926,12 @@
       <c r="AD87">
         <v>0.76852130744697178</v>
       </c>
-    </row>
-    <row r="88" spans="1:30">
+      <c r="AE87">
+        <f>AC87-1</f>
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:31">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -6731,7 +6961,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:30">
+    <row r="89" spans="1:31" hidden="1">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -6750,8 +6980,12 @@
       <c r="AD89">
         <v>0.12247448713915883</v>
       </c>
-    </row>
-    <row r="90" spans="1:30">
+      <c r="AE89">
+        <f>AC89-1</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:31" hidden="1">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -6788,8 +7022,12 @@
       <c r="AD90">
         <v>0.68328251843582888</v>
       </c>
-    </row>
-    <row r="91" spans="1:30">
+      <c r="AE90">
+        <f>AC90-1</f>
+        <v>12.049999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:31" hidden="1">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -6819,7 +7057,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:31" hidden="1">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -6838,8 +7076,12 @@
       <c r="AD92">
         <v>0.25860201081971496</v>
       </c>
-    </row>
-    <row r="93" spans="1:30">
+      <c r="AE92">
+        <f>AC92-1</f>
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:31" hidden="1">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -6876,8 +7118,12 @@
       <c r="AD93">
         <v>0.96136296475368743</v>
       </c>
-    </row>
-    <row r="94" spans="1:30">
+      <c r="AE93">
+        <f>AC93-1</f>
+        <v>5.9249999999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:31" hidden="1">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -6907,7 +7153,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:31" hidden="1">
       <c r="A95" t="s">
         <v>18</v>
       </c>
@@ -6926,8 +7172,12 @@
       <c r="AD95">
         <v>0.13479150566708564</v>
       </c>
-    </row>
-    <row r="96" spans="1:30">
+      <c r="AE95">
+        <f>AC95-1</f>
+        <v>4.335</v>
+      </c>
+    </row>
+    <row r="96" spans="1:31" hidden="1">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -6964,8 +7214,12 @@
       <c r="AD96">
         <v>0.91472331882378766</v>
       </c>
-    </row>
-    <row r="97" spans="1:30">
+      <c r="AE96">
+        <f>AC96-1</f>
+        <v>6.9249999999999989</v>
+      </c>
+    </row>
+    <row r="97" spans="1:31" hidden="1">
       <c r="A97" t="s">
         <v>18</v>
       </c>
@@ -6995,7 +7249,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:31" hidden="1">
       <c r="A98" t="s">
         <v>18</v>
       </c>
@@ -7014,8 +7268,12 @@
       <c r="AD98">
         <v>0.70887234393788967</v>
       </c>
-    </row>
-    <row r="99" spans="1:30">
+      <c r="AE98">
+        <f>AC98-1</f>
+        <v>4.8666666666666671</v>
+      </c>
+    </row>
+    <row r="99" spans="1:31" hidden="1">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -7052,8 +7310,12 @@
       <c r="AD99">
         <v>1.6416455159382026</v>
       </c>
-    </row>
-    <row r="100" spans="1:30">
+      <c r="AE99">
+        <f>AC99-1</f>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:31" hidden="1">
       <c r="A100" t="s">
         <v>18</v>
       </c>
@@ -7083,7 +7345,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:31" hidden="1">
       <c r="A101" t="s">
         <v>18</v>
       </c>
@@ -7102,8 +7364,12 @@
       <c r="AD101">
         <v>0.12990381056766589</v>
       </c>
-    </row>
-    <row r="102" spans="1:30">
+      <c r="AE101">
+        <f>AC101-1</f>
+        <v>3.8499999999999996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:31" hidden="1">
       <c r="A102" t="s">
         <v>18</v>
       </c>
@@ -7140,8 +7406,12 @@
       <c r="AD102">
         <v>0.48653751140071555</v>
       </c>
-    </row>
-    <row r="103" spans="1:30">
+      <c r="AE102">
+        <f>AC102-1</f>
+        <v>6.0749999999999993</v>
+      </c>
+    </row>
+    <row r="103" spans="1:31" hidden="1">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -7171,7 +7441,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:31">
       <c r="A104" t="s">
         <v>18</v>
       </c>
@@ -7203,13 +7473,17 @@
         <v>77</v>
       </c>
       <c r="AC104">
-        <v>6.6</v>
+        <v>7.3</v>
       </c>
       <c r="AD104">
-        <v>7.0710678118654655E-2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:30">
+        <v>1.0965856099730658</v>
+      </c>
+      <c r="AE104">
+        <f>AC104-1</f>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:31">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -7241,13 +7515,17 @@
         <v>77</v>
       </c>
       <c r="AC105">
-        <v>7.3</v>
+        <v>6.6</v>
       </c>
       <c r="AD105">
-        <v>1.0965856099730658</v>
-      </c>
-    </row>
-    <row r="106" spans="1:30">
+        <v>7.0710678118654655E-2</v>
+      </c>
+      <c r="AE105">
+        <f>AC105-1</f>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:31">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -7279,13 +7557,17 @@
         <v>77</v>
       </c>
       <c r="AC106">
-        <v>10.797499999999999</v>
+        <v>12.95</v>
       </c>
       <c r="AD106">
-        <v>1.1578664376775096</v>
-      </c>
-    </row>
-    <row r="107" spans="1:30">
+        <v>1.0280442597476069</v>
+      </c>
+      <c r="AE106">
+        <f>AC106-1</f>
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:31">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -7317,13 +7599,17 @@
         <v>77</v>
       </c>
       <c r="AC107">
-        <v>12.95</v>
+        <v>10.797499999999999</v>
       </c>
       <c r="AD107">
-        <v>1.0280442597476069</v>
-      </c>
-    </row>
-    <row r="108" spans="1:30">
+        <v>1.1578664376775096</v>
+      </c>
+      <c r="AE107">
+        <f>AC107-1</f>
+        <v>9.7974999999999994</v>
+      </c>
+    </row>
+    <row r="108" spans="1:31" hidden="1">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -7360,8 +7646,12 @@
       <c r="AD108">
         <v>0.42720018726587772</v>
       </c>
-    </row>
-    <row r="109" spans="1:30">
+      <c r="AE108">
+        <f t="shared" ref="AE106:AE151" si="4">AC108-1</f>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:31" hidden="1">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -7393,13 +7683,17 @@
         <v>74</v>
       </c>
       <c r="AC109">
-        <v>7.8000000000000007</v>
+        <v>10.350000000000001</v>
       </c>
       <c r="AD109">
-        <v>0.25495097567963915</v>
-      </c>
-    </row>
-    <row r="110" spans="1:30">
+        <v>1.1453711188955278</v>
+      </c>
+      <c r="AE109">
+        <f>AC109-1</f>
+        <v>9.3500000000000014</v>
+      </c>
+    </row>
+    <row r="110" spans="1:31" hidden="1">
       <c r="A110" t="s">
         <v>18</v>
       </c>
@@ -7431,13 +7725,17 @@
         <v>74</v>
       </c>
       <c r="AC110">
-        <v>10.350000000000001</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="AD110">
-        <v>1.1453711188955278</v>
-      </c>
-    </row>
-    <row r="111" spans="1:30">
+        <v>0.25495097567963915</v>
+      </c>
+      <c r="AE110">
+        <f>AC110-1</f>
+        <v>6.8000000000000007</v>
+      </c>
+    </row>
+    <row r="111" spans="1:31" hidden="1">
       <c r="A111" t="s">
         <v>18</v>
       </c>
@@ -7474,8 +7772,12 @@
       <c r="AD111">
         <v>0.73950997288745202</v>
       </c>
-    </row>
-    <row r="112" spans="1:30">
+      <c r="AE111">
+        <f t="shared" si="4"/>
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:31" hidden="1">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -7512,8 +7814,12 @@
       <c r="AD112">
         <v>0.31917863337009256</v>
       </c>
-    </row>
-    <row r="113" spans="1:30">
+      <c r="AE112">
+        <f t="shared" si="4"/>
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:31" hidden="1">
       <c r="A113" t="s">
         <v>18</v>
       </c>
@@ -7550,8 +7856,12 @@
       <c r="AD113">
         <v>0.42646805273080135</v>
       </c>
-    </row>
-    <row r="114" spans="1:30">
+      <c r="AE113">
+        <f t="shared" si="4"/>
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="114" spans="1:31" hidden="1">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -7583,13 +7893,17 @@
         <v>77</v>
       </c>
       <c r="AC114">
-        <v>10.734999999999999</v>
+        <v>11.6</v>
       </c>
       <c r="AD114">
-        <v>1.3066392960568749</v>
-      </c>
-    </row>
-    <row r="115" spans="1:30">
+        <v>0.25495097567963931</v>
+      </c>
+      <c r="AE114">
+        <f>AC114-1</f>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:31" hidden="1">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -7621,13 +7935,17 @@
         <v>77</v>
       </c>
       <c r="AC115">
-        <v>11.6</v>
+        <v>10.734999999999999</v>
       </c>
       <c r="AD115">
-        <v>0.25495097567963931</v>
-      </c>
-    </row>
-    <row r="116" spans="1:30">
+        <v>1.3066392960568749</v>
+      </c>
+      <c r="AE115">
+        <f>AC115-1</f>
+        <v>9.7349999999999994</v>
+      </c>
+    </row>
+    <row r="116" spans="1:31" hidden="1">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -7664,8 +7982,12 @@
       <c r="AD116">
         <v>0.26562295750848708</v>
       </c>
-    </row>
-    <row r="117" spans="1:30">
+      <c r="AE116">
+        <f t="shared" si="4"/>
+        <v>5.3666666666666671</v>
+      </c>
+    </row>
+    <row r="117" spans="1:31" hidden="1">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -7702,8 +8024,12 @@
       <c r="AD117">
         <v>4.330127018922178E-2</v>
       </c>
-    </row>
-    <row r="118" spans="1:30">
+      <c r="AE117">
+        <f t="shared" si="4"/>
+        <v>5.5500000000000007</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31" hidden="1">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -7735,13 +8061,17 @@
         <v>77</v>
       </c>
       <c r="AC118">
-        <v>9.5250000000000004</v>
+        <v>11.25</v>
       </c>
       <c r="AD118">
-        <v>1.1822991372744869</v>
-      </c>
-    </row>
-    <row r="119" spans="1:30">
+        <v>1.1233320969330469</v>
+      </c>
+      <c r="AE118">
+        <f>AC118-1</f>
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:31" hidden="1">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -7773,13 +8103,17 @@
         <v>77</v>
       </c>
       <c r="AC119">
-        <v>11.25</v>
+        <v>9.5250000000000004</v>
       </c>
       <c r="AD119">
-        <v>1.1233320969330469</v>
-      </c>
-    </row>
-    <row r="120" spans="1:30">
+        <v>1.1822991372744869</v>
+      </c>
+      <c r="AE119">
+        <f>AC119-1</f>
+        <v>8.5250000000000004</v>
+      </c>
+    </row>
+    <row r="120" spans="1:31" hidden="1">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -7811,13 +8145,17 @@
         <v>77</v>
       </c>
       <c r="AC120">
-        <v>8.3000000000000007</v>
+        <v>11.549999999999999</v>
       </c>
       <c r="AD120">
-        <v>0.35000000000000009</v>
-      </c>
-    </row>
-    <row r="121" spans="1:30">
+        <v>0.5117372372614678</v>
+      </c>
+      <c r="AE120">
+        <f>AC120-1</f>
+        <v>10.549999999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:31" hidden="1">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -7849,13 +8187,17 @@
         <v>77</v>
       </c>
       <c r="AC121">
-        <v>8.35</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="AD121">
-        <v>0.47631397208144094</v>
-      </c>
-    </row>
-    <row r="122" spans="1:30">
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="AE121">
+        <f>AC121-1</f>
+        <v>7.3000000000000007</v>
+      </c>
+    </row>
+    <row r="122" spans="1:31" hidden="1">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -7887,13 +8229,17 @@
         <v>77</v>
       </c>
       <c r="AC122">
-        <v>11.549999999999999</v>
+        <v>8.35</v>
       </c>
       <c r="AD122">
-        <v>0.5117372372614678</v>
-      </c>
-    </row>
-    <row r="123" spans="1:30">
+        <v>0.47631397208144094</v>
+      </c>
+      <c r="AE122">
+        <f>AC122-1</f>
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="123" spans="1:31" hidden="1">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -7930,8 +8276,12 @@
       <c r="AD123">
         <v>2.0425657884141697</v>
       </c>
-    </row>
-    <row r="124" spans="1:30">
+      <c r="AE123">
+        <f t="shared" si="4"/>
+        <v>14.59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:31" hidden="1">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -7968,8 +8318,12 @@
       <c r="AD124">
         <v>0.3112474899497184</v>
       </c>
-    </row>
-    <row r="125" spans="1:30">
+      <c r="AE124">
+        <f t="shared" si="4"/>
+        <v>5.4499999999999993</v>
+      </c>
+    </row>
+    <row r="125" spans="1:31" hidden="1">
       <c r="A125" t="s">
         <v>18</v>
       </c>
@@ -8006,8 +8360,12 @@
       <c r="AD125">
         <v>0.2165063509461097</v>
       </c>
-    </row>
-    <row r="126" spans="1:30">
+      <c r="AE125">
+        <f t="shared" si="4"/>
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="126" spans="1:31" hidden="1">
       <c r="A126" t="s">
         <v>18</v>
       </c>
@@ -8044,8 +8402,12 @@
       <c r="AD126">
         <v>1.2852528934026968</v>
       </c>
-    </row>
-    <row r="127" spans="1:30">
+      <c r="AE126">
+        <f t="shared" si="4"/>
+        <v>10.85</v>
+      </c>
+    </row>
+    <row r="127" spans="1:31" hidden="1">
       <c r="A127" t="s">
         <v>18</v>
       </c>
@@ -8082,8 +8444,12 @@
       <c r="AD127">
         <v>1.7997829730275812</v>
       </c>
-    </row>
-    <row r="128" spans="1:30">
+      <c r="AE127">
+        <f t="shared" si="4"/>
+        <v>11.324999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:31">
       <c r="A128" t="s">
         <v>18</v>
       </c>
@@ -8120,8 +8486,12 @@
       <c r="AD128">
         <v>0.4023369234857751</v>
       </c>
-    </row>
-    <row r="129" spans="1:30">
+      <c r="AE128">
+        <f t="shared" si="4"/>
+        <v>3.1500000000000004</v>
+      </c>
+    </row>
+    <row r="129" spans="1:31">
       <c r="A129" t="s">
         <v>18</v>
       </c>
@@ -8153,13 +8523,17 @@
         <v>86.75</v>
       </c>
       <c r="AC129">
-        <v>11.3</v>
+        <v>11.35</v>
       </c>
       <c r="AD129">
-        <v>0.40311288741492768</v>
-      </c>
-    </row>
-    <row r="130" spans="1:30">
+        <v>0.86998563206526625</v>
+      </c>
+      <c r="AE129">
+        <f>AC129-1</f>
+        <v>10.35</v>
+      </c>
+    </row>
+    <row r="130" spans="1:31">
       <c r="A130" t="s">
         <v>18</v>
       </c>
@@ -8191,13 +8565,17 @@
         <v>86.75</v>
       </c>
       <c r="AC130">
-        <v>11.35</v>
+        <v>11.4</v>
       </c>
       <c r="AD130">
-        <v>0.86998563206526625</v>
-      </c>
-    </row>
-    <row r="131" spans="1:30">
+        <v>0.59160797830996281</v>
+      </c>
+      <c r="AE130">
+        <f>AC130-1</f>
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:31">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -8229,13 +8607,17 @@
         <v>86.75</v>
       </c>
       <c r="AC131">
-        <v>11.4</v>
+        <v>11.3</v>
       </c>
       <c r="AD131">
-        <v>0.59160797830996281</v>
-      </c>
-    </row>
-    <row r="132" spans="1:30">
+        <v>0.40311288741492768</v>
+      </c>
+      <c r="AE131">
+        <f>AC131-1</f>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:31" hidden="1">
       <c r="A132" t="s">
         <v>18</v>
       </c>
@@ -8272,8 +8654,12 @@
       <c r="AD132">
         <v>0.2861380785564886</v>
       </c>
-    </row>
-    <row r="133" spans="1:30">
+      <c r="AE132">
+        <f t="shared" si="4"/>
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="133" spans="1:31" hidden="1">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -8305,13 +8691,17 @@
         <v>86</v>
       </c>
       <c r="AC133">
-        <v>6.75</v>
+        <v>14.8125</v>
       </c>
       <c r="AD133">
-        <v>0.57608593109014572</v>
-      </c>
-    </row>
-    <row r="134" spans="1:30">
+        <v>1.5370807355178191</v>
+      </c>
+      <c r="AE133">
+        <f>AC133-1</f>
+        <v>13.8125</v>
+      </c>
+    </row>
+    <row r="134" spans="1:31" hidden="1">
       <c r="A134" t="s">
         <v>18</v>
       </c>
@@ -8348,8 +8738,12 @@
       <c r="AD134">
         <v>1.6023420358962095</v>
       </c>
-    </row>
-    <row r="135" spans="1:30">
+      <c r="AE134">
+        <f t="shared" si="4"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:31" hidden="1">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -8381,13 +8775,17 @@
         <v>86</v>
       </c>
       <c r="AC135">
-        <v>14.8125</v>
+        <v>6.75</v>
       </c>
       <c r="AD135">
-        <v>1.5370807355178191</v>
-      </c>
-    </row>
-    <row r="136" spans="1:30">
+        <v>0.57608593109014572</v>
+      </c>
+      <c r="AE135">
+        <f>AC135-1</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="136" spans="1:31" hidden="1">
       <c r="A136" t="s">
         <v>18</v>
       </c>
@@ -8424,8 +8822,12 @@
       <c r="AD136">
         <v>0.18027756377320001</v>
       </c>
-    </row>
-    <row r="137" spans="1:30">
+      <c r="AE136">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:31" hidden="1">
       <c r="A137" t="s">
         <v>18</v>
       </c>
@@ -8457,13 +8859,17 @@
         <v>89</v>
       </c>
       <c r="AC137">
-        <v>8.2000000000000011</v>
+        <v>12.15</v>
       </c>
       <c r="AD137">
-        <v>0.25495097567963931</v>
-      </c>
-    </row>
-    <row r="138" spans="1:30">
+        <v>1.0520812706250384</v>
+      </c>
+      <c r="AE137">
+        <f>AC137-1</f>
+        <v>11.15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:31" hidden="1">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -8500,8 +8906,12 @@
       <c r="AD138">
         <v>0.54025456962435869</v>
       </c>
-    </row>
-    <row r="139" spans="1:30">
+      <c r="AE138">
+        <f>AC138-1</f>
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="139" spans="1:31" hidden="1">
       <c r="A139" t="s">
         <v>18</v>
       </c>
@@ -8533,13 +8943,17 @@
         <v>89</v>
       </c>
       <c r="AC139">
-        <v>12.15</v>
+        <v>8.2000000000000011</v>
       </c>
       <c r="AD139">
-        <v>1.0520812706250384</v>
-      </c>
-    </row>
-    <row r="140" spans="1:30">
+        <v>0.25495097567963931</v>
+      </c>
+      <c r="AE139">
+        <f>AC139-1</f>
+        <v>7.2000000000000011</v>
+      </c>
+    </row>
+    <row r="140" spans="1:31" hidden="1">
       <c r="A140" t="s">
         <v>18</v>
       </c>
@@ -8576,8 +8990,12 @@
       <c r="AD140">
         <v>0.38951091127207282</v>
       </c>
-    </row>
-    <row r="141" spans="1:30">
+      <c r="AE140">
+        <f t="shared" si="4"/>
+        <v>2.7249999999999996</v>
+      </c>
+    </row>
+    <row r="141" spans="1:31" hidden="1">
       <c r="A141" t="s">
         <v>18</v>
       </c>
@@ -8609,13 +9027,17 @@
         <v>89</v>
       </c>
       <c r="AC141">
-        <v>7.7</v>
+        <v>12.55</v>
       </c>
       <c r="AD141">
-        <v>0.43874821936960495</v>
-      </c>
-    </row>
-    <row r="142" spans="1:30">
+        <v>1.0825317547305451</v>
+      </c>
+      <c r="AE141">
+        <f>AC141-1</f>
+        <v>11.55</v>
+      </c>
+    </row>
+    <row r="142" spans="1:31" hidden="1">
       <c r="A142" t="s">
         <v>18</v>
       </c>
@@ -8647,13 +9069,17 @@
         <v>89</v>
       </c>
       <c r="AC142">
-        <v>10.6</v>
+        <v>7.7</v>
       </c>
       <c r="AD142">
-        <v>0.37416573867739411</v>
-      </c>
-    </row>
-    <row r="143" spans="1:30">
+        <v>0.43874821936960495</v>
+      </c>
+      <c r="AE142">
+        <f>AC142-1</f>
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:31" hidden="1">
       <c r="A143" t="s">
         <v>18</v>
       </c>
@@ -8685,13 +9111,17 @@
         <v>89</v>
       </c>
       <c r="AC143">
-        <v>12.55</v>
+        <v>10.6</v>
       </c>
       <c r="AD143">
-        <v>1.0825317547305451</v>
-      </c>
-    </row>
-    <row r="144" spans="1:30">
+        <v>0.37416573867739411</v>
+      </c>
+      <c r="AE143">
+        <f>AC143-1</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:31" hidden="1">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -8728,8 +9158,12 @@
       <c r="AD144">
         <v>0.20463381929681126</v>
       </c>
-    </row>
-    <row r="145" spans="1:30">
+      <c r="AE144">
+        <f t="shared" si="4"/>
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="145" spans="1:31" hidden="1">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -8761,13 +9195,17 @@
         <v>86</v>
       </c>
       <c r="AC145">
-        <v>8.375</v>
+        <v>14.825000000000001</v>
       </c>
       <c r="AD145">
-        <v>0.57268555944776545</v>
-      </c>
-    </row>
-    <row r="146" spans="1:30">
+        <v>0.81729355191387199</v>
+      </c>
+      <c r="AE145">
+        <f>AC145-1</f>
+        <v>13.825000000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:31" hidden="1">
       <c r="A146" t="s">
         <v>18</v>
       </c>
@@ -8799,13 +9237,17 @@
         <v>86</v>
       </c>
       <c r="AC146">
-        <v>12.95</v>
+        <v>8.375</v>
       </c>
       <c r="AD146">
-        <v>0.80738776309775961</v>
-      </c>
-    </row>
-    <row r="147" spans="1:30">
+        <v>0.57268555944776545</v>
+      </c>
+      <c r="AE146">
+        <f>AC146-1</f>
+        <v>7.375</v>
+      </c>
+    </row>
+    <row r="147" spans="1:31" hidden="1">
       <c r="A147" t="s">
         <v>18</v>
       </c>
@@ -8837,13 +9279,17 @@
         <v>86</v>
       </c>
       <c r="AC147">
-        <v>14.825000000000001</v>
+        <v>12.95</v>
       </c>
       <c r="AD147">
-        <v>0.81729355191387199</v>
-      </c>
-    </row>
-    <row r="148" spans="1:30">
+        <v>0.80738776309775961</v>
+      </c>
+      <c r="AE147">
+        <f>AC147-1</f>
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="148" spans="1:31" hidden="1">
       <c r="A148" t="s">
         <v>18</v>
       </c>
@@ -8880,8 +9326,12 @@
       <c r="AD148">
         <v>0.12247448713915901</v>
       </c>
-    </row>
-    <row r="149" spans="1:30">
+      <c r="AE148">
+        <f t="shared" si="4"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:31" hidden="1">
       <c r="A149" t="s">
         <v>18</v>
       </c>
@@ -8913,13 +9363,17 @@
         <v>88.25</v>
       </c>
       <c r="AC149">
-        <v>11.8</v>
+        <v>13.05</v>
       </c>
       <c r="AD149">
-        <v>1.0606601717798247</v>
-      </c>
-    </row>
-    <row r="150" spans="1:30">
+        <v>0.36314597615834865</v>
+      </c>
+      <c r="AE149">
+        <f>AC149-1</f>
+        <v>12.05</v>
+      </c>
+    </row>
+    <row r="150" spans="1:31" hidden="1">
       <c r="A150" t="s">
         <v>18</v>
       </c>
@@ -8951,13 +9405,17 @@
         <v>88.25</v>
       </c>
       <c r="AC150">
-        <v>13.05</v>
+        <v>13.75</v>
       </c>
       <c r="AD150">
-        <v>0.36314597615834865</v>
-      </c>
-    </row>
-    <row r="151" spans="1:30">
+        <v>1.6618889854620265</v>
+      </c>
+      <c r="AE150">
+        <f>AC150-1</f>
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="151" spans="1:31" hidden="1">
       <c r="A151" t="s">
         <v>18</v>
       </c>
@@ -8989,13 +9447,26 @@
         <v>88.25</v>
       </c>
       <c r="AC151">
-        <v>13.75</v>
+        <v>11.8</v>
       </c>
       <c r="AD151">
-        <v>1.6618889854620265</v>
+        <v>1.0606601717798247</v>
+      </c>
+      <c r="AE151">
+        <f>AC151-1</f>
+        <v>10.8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AE151" xr:uid="{1EE8BA1D-C516-4D8E-A81D-3534C605AA12}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TOSyear3SowNov20CvBerken"/>
+        <filter val="TOSyear3SowOct20CvBerken"/>
+        <filter val="TOSyear3SowSept20CvBerken"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD151">
     <sortCondition ref="B2:B151"/>
     <sortCondition ref="AC2:AC151"/>

</xml_diff>

<commit_message>
Adjusted branching and LAR to fit with Robertson et al. paper and Gatton researchers' understanding
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/TOSobserved.xlsx
+++ b/Prototypes/Mungbean/TOSobserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C397C1F-FC9E-4AFD-989A-E8DDF6929C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE8F4CA-A154-40F2-B3B1-D43678963626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -260,16 +260,16 @@
     <t>EndCanopyDevelopment</t>
   </si>
   <si>
-    <t>Soybean.AboVegatativeround.Wt</t>
-  </si>
-  <si>
-    <t>Soybean.AboVegatativeround.WtError</t>
-  </si>
-  <si>
     <t>Vegetative</t>
   </si>
   <si>
     <t>Soybean.Leaf.BranchNumber</t>
+  </si>
+  <si>
+    <t>Soybean.AboveGround.Wt</t>
+  </si>
+  <si>
+    <t>Soybean.AboveGround.WtError</t>
   </si>
 </sst>
 </file>
@@ -692,12 +692,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3519DD51-BED6-4262-8A50-4DB48CCAF26B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AE151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG128" sqref="AG128"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -705,8 +704,7 @@
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="28" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" customWidth="1"/>
+    <col min="5" max="29" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1" ht="45">
@@ -735,10 +733,10 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>6</v>
@@ -795,7 +793,7 @@
         <v>11</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>28</v>
@@ -804,7 +802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" hidden="1">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -862,11 +860,8 @@
       <c r="AA2">
         <v>57.25</v>
       </c>
-      <c r="AB2">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" hidden="1">
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -945,11 +940,8 @@
       <c r="AA3">
         <v>57.25</v>
       </c>
-      <c r="AB3">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" hidden="1">
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1007,11 +999,8 @@
       <c r="AA4">
         <v>57</v>
       </c>
-      <c r="AB4">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" hidden="1">
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1087,11 +1076,8 @@
       <c r="AA5">
         <v>57</v>
       </c>
-      <c r="AB5">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" hidden="1">
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1146,11 +1132,8 @@
       <c r="AA6">
         <v>77</v>
       </c>
-      <c r="AB6">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" hidden="1">
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1230,11 +1213,8 @@
       <c r="AA7">
         <v>77</v>
       </c>
-      <c r="AB7">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" hidden="1">
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1289,11 +1269,8 @@
       <c r="AA8">
         <v>76.25</v>
       </c>
-      <c r="AB8">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" hidden="1">
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1373,11 +1350,8 @@
       <c r="AA9">
         <v>76.25</v>
       </c>
-      <c r="AB9">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" hidden="1">
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1435,11 +1409,8 @@
       <c r="AA10">
         <v>56.5</v>
       </c>
-      <c r="AB10">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" hidden="1">
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1519,11 +1490,8 @@
       <c r="AA11">
         <v>56.5</v>
       </c>
-      <c r="AB11">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" hidden="1">
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1581,11 +1549,8 @@
       <c r="AA12">
         <v>55.75</v>
       </c>
-      <c r="AB12">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" hidden="1">
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1665,11 +1630,8 @@
       <c r="AA13">
         <v>55.75</v>
       </c>
-      <c r="AB13">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" hidden="1">
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1725,17 +1687,17 @@
         <v>73</v>
       </c>
       <c r="AC14">
-        <v>8.25</v>
+        <v>8.4</v>
       </c>
       <c r="AD14">
-        <v>0.41457809879442498</v>
+        <v>0.52796780204857408</v>
       </c>
       <c r="AE14">
         <f>AC14-1</f>
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" hidden="1">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1746,7 +1708,7 @@
         <v>43886</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15">
         <v>170.565</v>
@@ -1791,17 +1753,17 @@
         <v>73</v>
       </c>
       <c r="AC15">
-        <v>8.4</v>
+        <v>8.25</v>
       </c>
       <c r="AD15">
-        <v>0.52796780204857408</v>
+        <v>0.41457809879442498</v>
       </c>
       <c r="AE15">
         <f>AC15-1</f>
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" hidden="1">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1879,17 +1841,17 @@
         <v>73</v>
       </c>
       <c r="AC16">
-        <v>11.7</v>
+        <v>12.049999999999999</v>
       </c>
       <c r="AD16">
-        <v>0.71239034243875055</v>
+        <v>0.44370598373247128</v>
       </c>
       <c r="AE16">
-        <f t="shared" ref="AE16:AE38" si="0">AC16-1</f>
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" hidden="1">
+        <f>AC16-1</f>
+        <v>11.049999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1951,17 +1913,17 @@
         <v>73</v>
       </c>
       <c r="AC17">
-        <v>12.049999999999999</v>
+        <v>11.7</v>
       </c>
       <c r="AD17">
-        <v>0.44370598373247128</v>
+        <v>0.71239034243875055</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="0"/>
-        <v>11.049999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" s="9" customFormat="1" hidden="1">
+        <f>AC17-1</f>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" s="9" customFormat="1">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1972,7 +1934,7 @@
         <v>43886</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18">
         <v>150.8475</v>
@@ -2033,11 +1995,11 @@
         <v>0.58040933831219732</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AE18:AE38" si="0">AC18-1</f>
         <v>5.7499999999999991</v>
       </c>
     </row>
-    <row r="19" spans="1:31" s="9" customFormat="1" hidden="1">
+    <row r="19" spans="1:31" s="9" customFormat="1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2113,7 +2075,7 @@
         <v>7.0500000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:31" s="9" customFormat="1" hidden="1">
+    <row r="20" spans="1:31" s="9" customFormat="1">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2194,17 +2156,17 @@
         <v>73</v>
       </c>
       <c r="AC20">
-        <v>10.35</v>
+        <v>11.100000000000001</v>
       </c>
       <c r="AD20">
-        <v>0.24874685927665507</v>
+        <v>0.50249378105604425</v>
       </c>
       <c r="AE20">
-        <f t="shared" si="0"/>
-        <v>9.35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" s="9" customFormat="1" hidden="1">
+        <f>AC20-1</f>
+        <v>10.100000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" s="9" customFormat="1">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2274,17 +2236,17 @@
         <v>73</v>
       </c>
       <c r="AC21">
-        <v>11.100000000000001</v>
+        <v>10.35</v>
       </c>
       <c r="AD21">
-        <v>0.50249378105604425</v>
+        <v>0.24874685927665507</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="0"/>
-        <v>10.100000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" hidden="1">
+        <f>AC21-1</f>
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2295,7 +2257,7 @@
         <v>43878</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22">
         <v>35.647500000000001</v>
@@ -2350,7 +2312,7 @@
         <v>3.4499999999999993</v>
       </c>
     </row>
-    <row r="23" spans="1:31" hidden="1">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2416,7 +2378,7 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="24" spans="1:31" hidden="1">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2488,7 +2450,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="25" spans="1:31" hidden="1">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2576,7 +2538,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="26" spans="1:31" hidden="1">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2587,7 +2549,7 @@
         <v>43886</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E26">
         <v>119.9025</v>
@@ -2642,7 +2604,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="27" spans="1:31" hidden="1">
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -2708,7 +2670,7 @@
         <v>7.15</v>
       </c>
     </row>
-    <row r="28" spans="1:31" hidden="1">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -2786,17 +2748,17 @@
         <v>73</v>
       </c>
       <c r="AC28">
-        <v>10.7</v>
+        <v>11.15</v>
       </c>
       <c r="AD28">
-        <v>0.47696960070847289</v>
+        <v>8.2915619758885034E-2</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="0"/>
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" hidden="1">
+        <f>AC28-1</f>
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2858,17 +2820,17 @@
         <v>73</v>
       </c>
       <c r="AC29">
-        <v>11.15</v>
+        <v>10.7</v>
       </c>
       <c r="AD29">
-        <v>8.2915619758885034E-2</v>
+        <v>0.47696960070847289</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="0"/>
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" hidden="1">
+        <f>AC29-1</f>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -2879,7 +2841,7 @@
         <v>43878</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E30">
         <v>51.699999999999996</v>
@@ -2934,7 +2896,7 @@
         <v>5.1999999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:31" hidden="1">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2996,17 +2958,17 @@
         <v>69</v>
       </c>
       <c r="AC31">
-        <v>9.0500000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AD31">
-        <v>0.55396299515400349</v>
+        <v>0.70887234393788967</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="0"/>
-        <v>8.0500000000000007</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" hidden="1">
+        <f>AC31-1</f>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3062,17 +3024,17 @@
         <v>69</v>
       </c>
       <c r="AC32">
-        <v>9.3000000000000007</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="AD32">
-        <v>0.70887234393788967</v>
+        <v>0.55396299515400349</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="0"/>
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" hidden="1">
+        <f>AC32-1</f>
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -3160,7 +3122,7 @@
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:31" hidden="1">
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3171,7 +3133,7 @@
         <v>43886</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E34" s="9">
         <v>120.13</v>
@@ -3224,7 +3186,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="35" spans="1:31" hidden="1">
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -3300,7 +3262,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="36" spans="1:31" hidden="1">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -3368,7 +3330,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="37" spans="1:31" hidden="1">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -3459,7 +3421,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="38" spans="1:31" hidden="1">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -3531,7 +3493,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="39" spans="1:31" hidden="1">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -3542,7 +3504,7 @@
         <v>43829</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E39">
         <v>45.575000000000003</v>
@@ -3587,7 +3549,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:31" hidden="1">
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -3649,7 +3611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:31" hidden="1">
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -3727,7 +3689,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:31" hidden="1">
+    <row r="42" spans="1:31">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -3738,7 +3700,7 @@
         <v>43838</v>
       </c>
       <c r="D42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E42">
         <v>144.10750000000002</v>
@@ -3793,7 +3755,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="43" spans="1:31" hidden="1">
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -3865,7 +3827,7 @@
         <v>6.8999999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:31" hidden="1">
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -3943,17 +3905,17 @@
         <v>83</v>
       </c>
       <c r="AC44">
-        <v>11.875</v>
+        <v>14.85</v>
       </c>
       <c r="AD44">
-        <v>0.23284920012746457</v>
+        <v>0.49180788932264974</v>
       </c>
       <c r="AE44">
-        <f t="shared" ref="AE44:AE51" si="1">AC44-1</f>
-        <v>10.875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:31" hidden="1">
+        <f>AC44-1</f>
+        <v>13.85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -4015,17 +3977,17 @@
         <v>83</v>
       </c>
       <c r="AC45">
-        <v>14.85</v>
+        <v>11.875</v>
       </c>
       <c r="AD45">
-        <v>0.49180788932264974</v>
+        <v>0.23284920012746457</v>
       </c>
       <c r="AE45">
-        <f t="shared" si="1"/>
-        <v>13.85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:31" hidden="1">
+        <f>AC45-1</f>
+        <v>10.875</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -4036,7 +3998,7 @@
         <v>43838</v>
       </c>
       <c r="D46" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E46">
         <v>94.9</v>
@@ -4087,11 +4049,11 @@
         <v>0.47087020504593402</v>
       </c>
       <c r="AE46">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AE46:AE51" si="1">AC46-1</f>
         <v>4.2750000000000004</v>
       </c>
     </row>
-    <row r="47" spans="1:31" hidden="1">
+    <row r="47" spans="1:31">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -4163,7 +4125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:31" hidden="1">
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -4241,17 +4203,17 @@
         <v>83</v>
       </c>
       <c r="AC48">
-        <v>11.433333333333332</v>
+        <v>13.15</v>
       </c>
       <c r="AD48">
-        <v>0.22484562605386729</v>
+        <v>1.3141061600951396</v>
       </c>
       <c r="AE48">
-        <f t="shared" si="1"/>
-        <v>10.433333333333332</v>
-      </c>
-    </row>
-    <row r="49" spans="1:31" hidden="1">
+        <f>AC48-1</f>
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -4313,17 +4275,17 @@
         <v>83</v>
       </c>
       <c r="AC49">
-        <v>13.15</v>
+        <v>11.433333333333332</v>
       </c>
       <c r="AD49">
-        <v>1.3141061600951396</v>
+        <v>0.22484562605386729</v>
       </c>
       <c r="AE49">
-        <f t="shared" si="1"/>
-        <v>12.15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31" hidden="1">
+        <f>AC49-1</f>
+        <v>10.433333333333332</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -4334,7 +4296,7 @@
         <v>43829</v>
       </c>
       <c r="D50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E50">
         <v>56.282499999999999</v>
@@ -4389,7 +4351,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="51" spans="1:31" hidden="1">
+    <row r="51" spans="1:31">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -4461,7 +4423,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="52" spans="1:31" hidden="1">
+    <row r="52" spans="1:31">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -4523,7 +4485,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:31" hidden="1">
+    <row r="53" spans="1:31">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -4601,7 +4563,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:31" hidden="1">
+    <row r="54" spans="1:31">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -4673,7 +4635,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="55" spans="1:31" hidden="1">
+    <row r="55" spans="1:31">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -4751,17 +4713,17 @@
         <v>83</v>
       </c>
       <c r="AC55">
-        <v>12.475</v>
+        <v>13.525</v>
       </c>
       <c r="AD55">
-        <v>0.81499616563515842</v>
+        <v>0.28145825622994264</v>
       </c>
       <c r="AE55">
-        <f>AC55-1</f>
-        <v>11.475</v>
-      </c>
-    </row>
-    <row r="56" spans="1:31" hidden="1">
+        <f t="shared" ref="AE55" si="2">AC55-1</f>
+        <v>12.525</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -4823,17 +4785,17 @@
         <v>83</v>
       </c>
       <c r="AC56">
-        <v>13.525</v>
+        <v>12.475</v>
       </c>
       <c r="AD56">
-        <v>0.28145825622994264</v>
+        <v>0.81499616563515842</v>
       </c>
       <c r="AE56">
-        <f t="shared" ref="AE56" si="2">AC56-1</f>
-        <v>12.525</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31" hidden="1">
+        <f>AC56-1</f>
+        <v>11.475</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -4844,7 +4806,7 @@
         <v>43838</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E57">
         <v>123.60249999999999</v>
@@ -4889,7 +4851,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:31" hidden="1">
+    <row r="58" spans="1:31">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -4900,7 +4862,7 @@
         <v>43838</v>
       </c>
       <c r="D58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E58">
         <v>135.79250000000002</v>
@@ -4955,7 +4917,7 @@
         <v>4.4499999999999993</v>
       </c>
     </row>
-    <row r="59" spans="1:31" hidden="1">
+    <row r="59" spans="1:31">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -5027,7 +4989,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="60" spans="1:31" hidden="1">
+    <row r="60" spans="1:31">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -5105,17 +5067,17 @@
         <v>83</v>
       </c>
       <c r="AC60">
-        <v>11.899999999999999</v>
+        <v>14.65</v>
       </c>
       <c r="AD60">
-        <v>0.33541019662496857</v>
+        <v>1.3827056809024814</v>
       </c>
       <c r="AE60">
-        <f t="shared" ref="AE60:AE63" si="3">AC60-1</f>
-        <v>10.899999999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:31" hidden="1">
+        <f>AC60-1</f>
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -5177,17 +5139,17 @@
         <v>83</v>
       </c>
       <c r="AC61">
-        <v>14.65</v>
+        <v>11.899999999999999</v>
       </c>
       <c r="AD61">
-        <v>1.3827056809024814</v>
+        <v>0.33541019662496857</v>
       </c>
       <c r="AE61">
-        <f t="shared" si="3"/>
-        <v>13.65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:31" hidden="1">
+        <f>AC61-1</f>
+        <v>10.899999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -5255,11 +5217,11 @@
         <v>0.68590724591594887</v>
       </c>
       <c r="AE62">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AE62:AE63" si="3">AC62-1</f>
         <v>7.1749999999999989</v>
       </c>
     </row>
-    <row r="63" spans="1:31" hidden="1">
+    <row r="63" spans="1:31">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -5331,7 +5293,7 @@
         <v>12.400000000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:31" hidden="1">
+    <row r="64" spans="1:31">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -5342,7 +5304,7 @@
         <v>43788</v>
       </c>
       <c r="D64" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E64">
         <v>12.612500000000001</v>
@@ -5387,7 +5349,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:31" hidden="1">
+    <row r="65" spans="1:31">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -5465,7 +5427,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:31" hidden="1">
+    <row r="66" spans="1:31">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -5537,7 +5499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:31" hidden="1">
+    <row r="67" spans="1:31">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -5625,7 +5587,7 @@
         <v>7.3500000000000014</v>
       </c>
     </row>
-    <row r="68" spans="1:31" hidden="1">
+    <row r="68" spans="1:31">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -5636,7 +5598,7 @@
         <v>43795</v>
       </c>
       <c r="D68" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E68">
         <v>34.145000000000003</v>
@@ -5681,7 +5643,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:31" hidden="1">
+    <row r="69" spans="1:31">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -5743,7 +5705,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:31" hidden="1">
+    <row r="70" spans="1:31">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -5809,7 +5771,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="71" spans="1:31" hidden="1">
+    <row r="71" spans="1:31">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -5887,17 +5849,17 @@
         <v>91</v>
       </c>
       <c r="AC71">
-        <v>8</v>
+        <v>12.05</v>
       </c>
       <c r="AD71">
-        <v>0.71763500472036656</v>
+        <v>0.7595228765481663</v>
       </c>
       <c r="AE71">
         <f>AC71-1</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:31" hidden="1">
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -5959,17 +5921,17 @@
         <v>91</v>
       </c>
       <c r="AC72">
-        <v>12.05</v>
+        <v>8</v>
       </c>
       <c r="AD72">
-        <v>0.7595228765481663</v>
+        <v>0.71763500472036656</v>
       </c>
       <c r="AE72">
         <f>AC72-1</f>
-        <v>11.05</v>
-      </c>
-    </row>
-    <row r="73" spans="1:31" hidden="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -5980,7 +5942,7 @@
         <v>43795</v>
       </c>
       <c r="D73" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E73">
         <v>31.502499999999998</v>
@@ -6025,7 +5987,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:31" hidden="1">
+    <row r="74" spans="1:31">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -6087,17 +6049,17 @@
         <v>84</v>
       </c>
       <c r="AC74">
-        <v>5.75</v>
+        <v>6.3250000000000002</v>
       </c>
       <c r="AD74">
-        <v>0.59319052588523336</v>
+        <v>0.81192287195274837</v>
       </c>
       <c r="AE74">
         <f>AC74-1</f>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="75" spans="1:31" hidden="1">
+        <v>5.3250000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -6159,17 +6121,17 @@
         <v>84</v>
       </c>
       <c r="AC75">
-        <v>6.3250000000000002</v>
+        <v>5.75</v>
       </c>
       <c r="AD75">
-        <v>0.81192287195274837</v>
+        <v>0.59319052588523336</v>
       </c>
       <c r="AE75">
         <f>AC75-1</f>
-        <v>5.3250000000000002</v>
-      </c>
-    </row>
-    <row r="76" spans="1:31" hidden="1">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31">
       <c r="A76" t="s">
         <v>18</v>
       </c>
@@ -6180,7 +6142,7 @@
         <v>43788</v>
       </c>
       <c r="D76" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E76">
         <v>15.4725</v>
@@ -6225,7 +6187,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:31" hidden="1">
+    <row r="77" spans="1:31">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -6303,7 +6265,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:31" hidden="1">
+    <row r="78" spans="1:31">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -6375,7 +6337,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:31" hidden="1">
+    <row r="79" spans="1:31">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -6463,7 +6425,7 @@
         <v>5.0250000000000004</v>
       </c>
     </row>
-    <row r="80" spans="1:31" hidden="1">
+    <row r="80" spans="1:31">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -6474,7 +6436,7 @@
         <v>43795</v>
       </c>
       <c r="D80" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E80">
         <v>45.987500000000004</v>
@@ -6519,7 +6481,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:31" hidden="1">
+    <row r="81" spans="1:31">
       <c r="A81" t="s">
         <v>18</v>
       </c>
@@ -6581,7 +6543,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:31" hidden="1">
+    <row r="82" spans="1:31">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -6647,7 +6609,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="83" spans="1:31" hidden="1">
+    <row r="83" spans="1:31">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -6725,17 +6687,17 @@
         <v>91</v>
       </c>
       <c r="AC83">
-        <v>7.15</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="AD83">
-        <v>0.24874685927665491</v>
+        <v>0.58309518948452843</v>
       </c>
       <c r="AE83">
         <f>AC83-1</f>
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:31" hidden="1">
+        <v>6.8000000000000007</v>
+      </c>
+    </row>
+    <row r="84" spans="1:31">
       <c r="A84" t="s">
         <v>18</v>
       </c>
@@ -6797,17 +6759,17 @@
         <v>91</v>
       </c>
       <c r="AC84">
-        <v>7.8000000000000007</v>
+        <v>7.15</v>
       </c>
       <c r="AD84">
-        <v>0.58309518948452843</v>
+        <v>0.24874685927665491</v>
       </c>
       <c r="AE84">
         <f>AC84-1</f>
-        <v>6.8000000000000007</v>
-      </c>
-    </row>
-    <row r="85" spans="1:31" hidden="1">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:31">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -6818,7 +6780,7 @@
         <v>43795</v>
       </c>
       <c r="D85" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E85">
         <v>30.85</v>
@@ -6874,7 +6836,7 @@
         <v>44182</v>
       </c>
       <c r="D86" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="S86" s="9"/>
       <c r="T86" s="9"/>
@@ -6961,7 +6923,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:31" hidden="1">
+    <row r="89" spans="1:31">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -6972,7 +6934,7 @@
         <v>44182</v>
       </c>
       <c r="D89" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC89">
         <v>5.4</v>
@@ -6985,7 +6947,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="90" spans="1:31" hidden="1">
+    <row r="90" spans="1:31">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -7027,7 +6989,7 @@
         <v>12.049999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:31" hidden="1">
+    <row r="91" spans="1:31">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -7057,7 +7019,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:31" hidden="1">
+    <row r="92" spans="1:31">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -7068,7 +7030,7 @@
         <v>44182</v>
       </c>
       <c r="D92" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC92">
         <v>5.15</v>
@@ -7081,7 +7043,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="93" spans="1:31" hidden="1">
+    <row r="93" spans="1:31">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -7123,7 +7085,7 @@
         <v>5.9249999999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:31" hidden="1">
+    <row r="94" spans="1:31">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -7153,7 +7115,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="95" spans="1:31" hidden="1">
+    <row r="95" spans="1:31">
       <c r="A95" t="s">
         <v>18</v>
       </c>
@@ -7164,7 +7126,7 @@
         <v>44182</v>
       </c>
       <c r="D95" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC95">
         <v>5.335</v>
@@ -7177,7 +7139,7 @@
         <v>4.335</v>
       </c>
     </row>
-    <row r="96" spans="1:31" hidden="1">
+    <row r="96" spans="1:31">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -7219,7 +7181,7 @@
         <v>6.9249999999999989</v>
       </c>
     </row>
-    <row r="97" spans="1:31" hidden="1">
+    <row r="97" spans="1:31">
       <c r="A97" t="s">
         <v>18</v>
       </c>
@@ -7249,7 +7211,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="98" spans="1:31" hidden="1">
+    <row r="98" spans="1:31">
       <c r="A98" t="s">
         <v>18</v>
       </c>
@@ -7260,7 +7222,7 @@
         <v>44182</v>
       </c>
       <c r="D98" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC98">
         <v>5.8666666666666671</v>
@@ -7273,7 +7235,7 @@
         <v>4.8666666666666671</v>
       </c>
     </row>
-    <row r="99" spans="1:31" hidden="1">
+    <row r="99" spans="1:31">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -7315,7 +7277,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="100" spans="1:31" hidden="1">
+    <row r="100" spans="1:31">
       <c r="A100" t="s">
         <v>18</v>
       </c>
@@ -7345,7 +7307,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="1:31" hidden="1">
+    <row r="101" spans="1:31">
       <c r="A101" t="s">
         <v>18</v>
       </c>
@@ -7356,7 +7318,7 @@
         <v>44182</v>
       </c>
       <c r="D101" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC101">
         <v>4.8499999999999996</v>
@@ -7369,7 +7331,7 @@
         <v>3.8499999999999996</v>
       </c>
     </row>
-    <row r="102" spans="1:31" hidden="1">
+    <row r="102" spans="1:31">
       <c r="A102" t="s">
         <v>18</v>
       </c>
@@ -7411,7 +7373,7 @@
         <v>6.0749999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:31" hidden="1">
+    <row r="103" spans="1:31">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -7494,7 +7456,7 @@
         <v>44158</v>
       </c>
       <c r="D105" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W105">
         <v>47</v>
@@ -7609,7 +7571,7 @@
         <v>9.7974999999999994</v>
       </c>
     </row>
-    <row r="108" spans="1:31" hidden="1">
+    <row r="108" spans="1:31">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -7620,7 +7582,7 @@
         <v>44158</v>
       </c>
       <c r="D108" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W108">
         <v>46</v>
@@ -7647,11 +7609,11 @@
         <v>0.42720018726587772</v>
       </c>
       <c r="AE108">
-        <f t="shared" ref="AE106:AE151" si="4">AC108-1</f>
+        <f t="shared" ref="AE108:AE148" si="4">AC108-1</f>
         <v>5.7</v>
       </c>
     </row>
-    <row r="109" spans="1:31" hidden="1">
+    <row r="109" spans="1:31">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -7693,7 +7655,7 @@
         <v>9.3500000000000014</v>
       </c>
     </row>
-    <row r="110" spans="1:31" hidden="1">
+    <row r="110" spans="1:31">
       <c r="A110" t="s">
         <v>18</v>
       </c>
@@ -7735,7 +7697,7 @@
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="111" spans="1:31" hidden="1">
+    <row r="111" spans="1:31">
       <c r="A111" t="s">
         <v>18</v>
       </c>
@@ -7777,7 +7739,7 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="112" spans="1:31" hidden="1">
+    <row r="112" spans="1:31">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -7819,7 +7781,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="113" spans="1:31" hidden="1">
+    <row r="113" spans="1:31">
       <c r="A113" t="s">
         <v>18</v>
       </c>
@@ -7830,7 +7792,7 @@
         <v>44158</v>
       </c>
       <c r="D113" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W113">
         <v>47</v>
@@ -7861,7 +7823,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="114" spans="1:31" hidden="1">
+    <row r="114" spans="1:31">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -7903,7 +7865,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="115" spans="1:31" hidden="1">
+    <row r="115" spans="1:31">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -7945,7 +7907,7 @@
         <v>9.7349999999999994</v>
       </c>
     </row>
-    <row r="116" spans="1:31" hidden="1">
+    <row r="116" spans="1:31">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -7956,7 +7918,7 @@
         <v>44158</v>
       </c>
       <c r="D116" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W116">
         <v>46.5</v>
@@ -7987,7 +7949,7 @@
         <v>5.3666666666666671</v>
       </c>
     </row>
-    <row r="117" spans="1:31" hidden="1">
+    <row r="117" spans="1:31">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -8029,7 +7991,7 @@
         <v>5.5500000000000007</v>
       </c>
     </row>
-    <row r="118" spans="1:31" hidden="1">
+    <row r="118" spans="1:31">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -8071,7 +8033,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="119" spans="1:31" hidden="1">
+    <row r="119" spans="1:31">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -8113,7 +8075,7 @@
         <v>8.5250000000000004</v>
       </c>
     </row>
-    <row r="120" spans="1:31" hidden="1">
+    <row r="120" spans="1:31">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -8155,7 +8117,7 @@
         <v>10.549999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:31" hidden="1">
+    <row r="121" spans="1:31">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -8166,7 +8128,7 @@
         <v>44158</v>
       </c>
       <c r="D121" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W121">
         <v>46</v>
@@ -8197,7 +8159,7 @@
         <v>7.3000000000000007</v>
       </c>
     </row>
-    <row r="122" spans="1:31" hidden="1">
+    <row r="122" spans="1:31">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -8239,7 +8201,7 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="123" spans="1:31" hidden="1">
+    <row r="123" spans="1:31">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -8281,7 +8243,7 @@
         <v>14.59</v>
       </c>
     </row>
-    <row r="124" spans="1:31" hidden="1">
+    <row r="124" spans="1:31">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -8292,7 +8254,7 @@
         <v>44158</v>
       </c>
       <c r="D124" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W124">
         <v>47</v>
@@ -8323,7 +8285,7 @@
         <v>5.4499999999999993</v>
       </c>
     </row>
-    <row r="125" spans="1:31" hidden="1">
+    <row r="125" spans="1:31">
       <c r="A125" t="s">
         <v>18</v>
       </c>
@@ -8365,7 +8327,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="126" spans="1:31" hidden="1">
+    <row r="126" spans="1:31">
       <c r="A126" t="s">
         <v>18</v>
       </c>
@@ -8407,7 +8369,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="127" spans="1:31" hidden="1">
+    <row r="127" spans="1:31">
       <c r="A127" t="s">
         <v>18</v>
       </c>
@@ -8460,7 +8422,7 @@
         <v>44117</v>
       </c>
       <c r="D128" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W128">
         <v>57</v>
@@ -8617,7 +8579,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="132" spans="1:31" hidden="1">
+    <row r="132" spans="1:31">
       <c r="A132" t="s">
         <v>18</v>
       </c>
@@ -8628,7 +8590,7 @@
         <v>44117</v>
       </c>
       <c r="D132" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W132">
         <v>48</v>
@@ -8659,7 +8621,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="133" spans="1:31" hidden="1">
+    <row r="133" spans="1:31">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -8701,7 +8663,7 @@
         <v>13.8125</v>
       </c>
     </row>
-    <row r="134" spans="1:31" hidden="1">
+    <row r="134" spans="1:31">
       <c r="A134" t="s">
         <v>18</v>
       </c>
@@ -8743,7 +8705,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="135" spans="1:31" hidden="1">
+    <row r="135" spans="1:31">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -8785,7 +8747,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="136" spans="1:31" hidden="1">
+    <row r="136" spans="1:31">
       <c r="A136" t="s">
         <v>18</v>
       </c>
@@ -8796,7 +8758,7 @@
         <v>44117</v>
       </c>
       <c r="D136" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W136">
         <v>58</v>
@@ -8827,7 +8789,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="137" spans="1:31" hidden="1">
+    <row r="137" spans="1:31">
       <c r="A137" t="s">
         <v>18</v>
       </c>
@@ -8869,7 +8831,7 @@
         <v>11.15</v>
       </c>
     </row>
-    <row r="138" spans="1:31" hidden="1">
+    <row r="138" spans="1:31">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -8911,7 +8873,7 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="139" spans="1:31" hidden="1">
+    <row r="139" spans="1:31">
       <c r="A139" t="s">
         <v>18</v>
       </c>
@@ -8953,7 +8915,7 @@
         <v>7.2000000000000011</v>
       </c>
     </row>
-    <row r="140" spans="1:31" hidden="1">
+    <row r="140" spans="1:31">
       <c r="A140" t="s">
         <v>18</v>
       </c>
@@ -8964,7 +8926,7 @@
         <v>44117</v>
       </c>
       <c r="D140" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W140">
         <v>50.25</v>
@@ -8995,7 +8957,7 @@
         <v>2.7249999999999996</v>
       </c>
     </row>
-    <row r="141" spans="1:31" hidden="1">
+    <row r="141" spans="1:31">
       <c r="A141" t="s">
         <v>18</v>
       </c>
@@ -9037,7 +8999,7 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="142" spans="1:31" hidden="1">
+    <row r="142" spans="1:31">
       <c r="A142" t="s">
         <v>18</v>
       </c>
@@ -9079,7 +9041,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="143" spans="1:31" hidden="1">
+    <row r="143" spans="1:31">
       <c r="A143" t="s">
         <v>18</v>
       </c>
@@ -9121,7 +9083,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="144" spans="1:31" hidden="1">
+    <row r="144" spans="1:31">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -9132,7 +9094,7 @@
         <v>44117</v>
       </c>
       <c r="D144" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W144">
         <v>48</v>
@@ -9163,7 +9125,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="145" spans="1:31" hidden="1">
+    <row r="145" spans="1:31">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -9205,7 +9167,7 @@
         <v>13.825000000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:31" hidden="1">
+    <row r="146" spans="1:31">
       <c r="A146" t="s">
         <v>18</v>
       </c>
@@ -9247,7 +9209,7 @@
         <v>7.375</v>
       </c>
     </row>
-    <row r="147" spans="1:31" hidden="1">
+    <row r="147" spans="1:31">
       <c r="A147" t="s">
         <v>18</v>
       </c>
@@ -9289,7 +9251,7 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="148" spans="1:31" hidden="1">
+    <row r="148" spans="1:31">
       <c r="A148" t="s">
         <v>18</v>
       </c>
@@ -9300,7 +9262,7 @@
         <v>44117</v>
       </c>
       <c r="D148" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="W148">
         <v>49.5</v>
@@ -9331,7 +9293,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="149" spans="1:31" hidden="1">
+    <row r="149" spans="1:31">
       <c r="A149" t="s">
         <v>18</v>
       </c>
@@ -9373,7 +9335,7 @@
         <v>12.05</v>
       </c>
     </row>
-    <row r="150" spans="1:31" hidden="1">
+    <row r="150" spans="1:31">
       <c r="A150" t="s">
         <v>18</v>
       </c>
@@ -9415,7 +9377,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="151" spans="1:31" hidden="1">
+    <row r="151" spans="1:31">
       <c r="A151" t="s">
         <v>18</v>
       </c>
@@ -9458,15 +9420,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE151" xr:uid="{1EE8BA1D-C516-4D8E-A81D-3534C605AA12}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TOSyear3SowNov20CvBerken"/>
-        <filter val="TOSyear3SowOct20CvBerken"/>
-        <filter val="TOSyear3SowSept20CvBerken"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD151">
     <sortCondition ref="B2:B151"/>
     <sortCondition ref="AC2:AC151"/>

</xml_diff>

<commit_message>
TOS 3 added in and Jade recalibrated.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/TOSobserved.xlsx
+++ b/Prototypes/Mungbean/TOSobserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C31BBD-FE5D-47AB-A5C7-2E0829F6297A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD3CC35-374F-4161-9E36-CC23DBAE45EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -537,6 +537,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,20 +859,18 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AL338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F226" sqref="F226"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V298" sqref="V298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" style="24" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" style="24" customWidth="1"/>
     <col min="6" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="24" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="25" max="36" width="9.140625" customWidth="1"/>
+    <col min="10" max="36" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="1" customFormat="1" ht="45">
@@ -879,7 +880,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="23" t="s">
@@ -10875,7 +10876,7 @@
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="219" spans="1:38">
+    <row r="219" spans="1:38" hidden="1">
       <c r="A219" t="s">
         <v>14</v>
       </c>
@@ -10940,7 +10941,7 @@
         <v>4.5500000000000007</v>
       </c>
     </row>
-    <row r="220" spans="1:38">
+    <row r="220" spans="1:38" hidden="1">
       <c r="A220" t="s">
         <v>14</v>
       </c>
@@ -11023,14 +11024,16 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="221" spans="1:38">
+    <row r="221" spans="1:38" hidden="1">
       <c r="A221" t="s">
         <v>14</v>
       </c>
       <c r="B221" t="s">
         <v>48</v>
       </c>
-      <c r="C221" s="7"/>
+      <c r="C221" s="7">
+        <v>44214</v>
+      </c>
       <c r="E221" s="31"/>
       <c r="F221" t="s">
         <v>67</v>
@@ -11078,7 +11081,9 @@
       <c r="B222" t="s">
         <v>48</v>
       </c>
-      <c r="C222" s="7"/>
+      <c r="C222" s="7">
+        <v>44225</v>
+      </c>
       <c r="E222" s="31"/>
       <c r="F222" t="s">
         <v>12</v>
@@ -11110,6 +11115,13 @@
       <c r="Q222">
         <v>0.37140519622151713</v>
       </c>
+      <c r="V222">
+        <v>1411.2125000000001</v>
+      </c>
+      <c r="W222">
+        <f>310/2</f>
+        <v>155</v>
+      </c>
       <c r="Y222">
         <v>238.18625</v>
       </c>
@@ -11136,7 +11148,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="223" spans="1:38">
+    <row r="223" spans="1:38" hidden="1">
       <c r="A223" t="s">
         <v>14</v>
       </c>
@@ -11200,7 +11212,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="224" spans="1:38">
+    <row r="224" spans="1:38" hidden="1">
       <c r="A224" t="s">
         <v>14</v>
       </c>
@@ -11282,14 +11294,16 @@
         <v>12.049999999999999</v>
       </c>
     </row>
-    <row r="225" spans="1:38">
+    <row r="225" spans="1:38" hidden="1">
       <c r="A225" t="s">
         <v>14</v>
       </c>
       <c r="B225" t="s">
         <v>49</v>
       </c>
-      <c r="C225" s="7"/>
+      <c r="C225" s="7">
+        <v>44210</v>
+      </c>
       <c r="E225" s="31"/>
       <c r="F225" t="s">
         <v>67</v>
@@ -11336,7 +11350,9 @@
       <c r="B226" t="s">
         <v>49</v>
       </c>
-      <c r="C226" s="7"/>
+      <c r="C226" s="7">
+        <v>44225</v>
+      </c>
       <c r="E226" s="31"/>
       <c r="F226" t="s">
         <v>12</v>
@@ -11368,6 +11384,13 @@
       <c r="Q226">
         <v>0.15691388191552219</v>
       </c>
+      <c r="V226">
+        <v>1122.5</v>
+      </c>
+      <c r="W226">
+        <f>167/2</f>
+        <v>83.5</v>
+      </c>
       <c r="Y226">
         <v>208.48166666666668</v>
       </c>
@@ -11394,7 +11417,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="227" spans="1:38">
+    <row r="227" spans="1:38" hidden="1">
       <c r="A227" t="s">
         <v>14</v>
       </c>
@@ -11458,7 +11481,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="228" spans="1:38">
+    <row r="228" spans="1:38" hidden="1">
       <c r="A228" t="s">
         <v>14</v>
       </c>
@@ -11540,14 +11563,16 @@
         <v>5.9249999999999998</v>
       </c>
     </row>
-    <row r="229" spans="1:38">
+    <row r="229" spans="1:38" hidden="1">
       <c r="A229" t="s">
         <v>14</v>
       </c>
       <c r="B229" t="s">
         <v>50</v>
       </c>
-      <c r="C229" s="7"/>
+      <c r="C229" s="7">
+        <v>44214</v>
+      </c>
       <c r="E229" s="31"/>
       <c r="F229" t="s">
         <v>67</v>
@@ -11594,7 +11619,9 @@
       <c r="B230" t="s">
         <v>50</v>
       </c>
-      <c r="C230" s="7"/>
+      <c r="C230" s="7">
+        <v>44232</v>
+      </c>
       <c r="E230" s="31"/>
       <c r="F230" t="s">
         <v>12</v>
@@ -11626,6 +11653,13 @@
       <c r="Q230">
         <v>0.19158441531463238</v>
       </c>
+      <c r="V230">
+        <v>1422.3</v>
+      </c>
+      <c r="W230">
+        <f>261.9/2</f>
+        <v>130.94999999999999</v>
+      </c>
       <c r="Y230">
         <v>211.34375</v>
       </c>
@@ -11652,7 +11686,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="231" spans="1:38">
+    <row r="231" spans="1:38" hidden="1">
       <c r="A231" t="s">
         <v>14</v>
       </c>
@@ -11716,7 +11750,7 @@
         <v>4.335</v>
       </c>
     </row>
-    <row r="232" spans="1:38">
+    <row r="232" spans="1:38" hidden="1">
       <c r="A232" t="s">
         <v>14</v>
       </c>
@@ -11798,14 +11832,16 @@
         <v>6.9249999999999989</v>
       </c>
     </row>
-    <row r="233" spans="1:38">
+    <row r="233" spans="1:38" hidden="1">
       <c r="A233" t="s">
         <v>14</v>
       </c>
       <c r="B233" t="s">
         <v>51</v>
       </c>
-      <c r="C233" s="7"/>
+      <c r="C233" s="7">
+        <v>44214</v>
+      </c>
       <c r="E233" s="31"/>
       <c r="F233" t="s">
         <v>67</v>
@@ -11852,7 +11888,9 @@
       <c r="B234" t="s">
         <v>51</v>
       </c>
-      <c r="C234" s="19"/>
+      <c r="C234" s="7">
+        <v>44232</v>
+      </c>
       <c r="D234" s="30"/>
       <c r="E234" s="37"/>
       <c r="F234" t="s">
@@ -11885,6 +11923,13 @@
       <c r="Q234">
         <v>7.0819146580885062E-2</v>
       </c>
+      <c r="V234">
+        <v>1061.54</v>
+      </c>
+      <c r="W234">
+        <f>297.7/2</f>
+        <v>148.85</v>
+      </c>
       <c r="Y234">
         <v>197.26374999999999</v>
       </c>
@@ -11910,7 +11955,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="235" spans="1:38">
+    <row r="235" spans="1:38" hidden="1">
       <c r="A235" t="s">
         <v>14</v>
       </c>
@@ -11973,7 +12018,7 @@
         <v>4.8666666666666671</v>
       </c>
     </row>
-    <row r="236" spans="1:38">
+    <row r="236" spans="1:38" hidden="1">
       <c r="A236" t="s">
         <v>14</v>
       </c>
@@ -12054,14 +12099,16 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="237" spans="1:38">
+    <row r="237" spans="1:38" hidden="1">
       <c r="A237" t="s">
         <v>14</v>
       </c>
       <c r="B237" t="s">
         <v>52</v>
       </c>
-      <c r="C237" s="19"/>
+      <c r="C237" s="7">
+        <v>44216</v>
+      </c>
       <c r="D237" s="30"/>
       <c r="E237" s="37"/>
       <c r="F237" t="s">
@@ -12108,7 +12155,9 @@
       <c r="B238" t="s">
         <v>52</v>
       </c>
-      <c r="C238" s="19"/>
+      <c r="C238" s="7">
+        <v>44235</v>
+      </c>
       <c r="D238" s="30"/>
       <c r="E238" s="37"/>
       <c r="F238" t="s">
@@ -12141,6 +12190,13 @@
       <c r="Q238">
         <v>0.18331549480837259</v>
       </c>
+      <c r="V238">
+        <v>595</v>
+      </c>
+      <c r="W238">
+        <f>224/2</f>
+        <v>112</v>
+      </c>
       <c r="Y238">
         <v>173.05916666666667</v>
       </c>
@@ -12166,7 +12222,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="239" spans="1:38">
+    <row r="239" spans="1:38" hidden="1">
       <c r="A239" t="s">
         <v>14</v>
       </c>
@@ -12229,7 +12285,7 @@
         <v>3.8499999999999996</v>
       </c>
     </row>
-    <row r="240" spans="1:38">
+    <row r="240" spans="1:38" hidden="1">
       <c r="A240" t="s">
         <v>14</v>
       </c>
@@ -12310,14 +12366,16 @@
         <v>6.0749999999999993</v>
       </c>
     </row>
-    <row r="241" spans="1:38">
+    <row r="241" spans="1:38" hidden="1">
       <c r="A241" t="s">
         <v>14</v>
       </c>
       <c r="B241" t="s">
         <v>53</v>
       </c>
-      <c r="C241" s="19"/>
+      <c r="C241" s="7">
+        <v>44214</v>
+      </c>
       <c r="D241" s="30"/>
       <c r="E241" s="37"/>
       <c r="F241" t="s">
@@ -12364,7 +12422,9 @@
       <c r="B242" t="s">
         <v>53</v>
       </c>
-      <c r="C242" s="19"/>
+      <c r="C242" s="7">
+        <v>44229</v>
+      </c>
       <c r="D242" s="30"/>
       <c r="E242" s="37"/>
       <c r="F242" t="s">
@@ -12397,6 +12457,13 @@
       <c r="Q242">
         <v>0.37906990625783948</v>
       </c>
+      <c r="V242">
+        <v>1155</v>
+      </c>
+      <c r="W242">
+        <f>188.8/2</f>
+        <v>94.4</v>
+      </c>
       <c r="Y242">
         <v>214.46666666666664</v>
       </c>
@@ -12422,7 +12489,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="243" spans="1:38">
+    <row r="243" spans="1:38" hidden="1">
       <c r="A243" t="s">
         <v>14</v>
       </c>
@@ -12503,7 +12570,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="244" spans="1:38">
+    <row r="244" spans="1:38" hidden="1">
       <c r="A244" t="s">
         <v>14</v>
       </c>
@@ -12592,7 +12659,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="245" spans="1:38">
+    <row r="245" spans="1:38" hidden="1">
       <c r="A245" t="s">
         <v>14</v>
       </c>
@@ -12719,6 +12786,13 @@
       <c r="Q246">
         <v>0.26160615917091551</v>
       </c>
+      <c r="V246">
+        <v>924.65</v>
+      </c>
+      <c r="W246">
+        <f>333.8/2</f>
+        <v>166.9</v>
+      </c>
       <c r="Y246">
         <v>228.15583333333333</v>
       </c>
@@ -12754,7 +12828,7 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="247" spans="1:38">
+    <row r="247" spans="1:38" hidden="1">
       <c r="A247" t="s">
         <v>14</v>
       </c>
@@ -12835,7 +12909,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="248" spans="1:38">
+    <row r="248" spans="1:38" hidden="1">
       <c r="A248" t="s">
         <v>14</v>
       </c>
@@ -12924,7 +12998,7 @@
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="249" spans="1:38">
+    <row r="249" spans="1:38" hidden="1">
       <c r="A249" t="s">
         <v>14</v>
       </c>
@@ -13051,6 +13125,13 @@
       <c r="Q250">
         <v>0.24229176713436737</v>
       </c>
+      <c r="V250">
+        <v>623.48</v>
+      </c>
+      <c r="W250">
+        <f>136.3/2</f>
+        <v>68.150000000000006</v>
+      </c>
       <c r="Y250">
         <v>252.66833333333332</v>
       </c>
@@ -13086,7 +13167,7 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="251" spans="1:38">
+    <row r="251" spans="1:38" hidden="1">
       <c r="A251" t="s">
         <v>14</v>
       </c>
@@ -13167,7 +13248,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="252" spans="1:38">
+    <row r="252" spans="1:38" hidden="1">
       <c r="A252" t="s">
         <v>14</v>
       </c>
@@ -13256,7 +13337,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="253" spans="1:38">
+    <row r="253" spans="1:38" hidden="1">
       <c r="A253" t="s">
         <v>14</v>
       </c>
@@ -13383,6 +13464,13 @@
       <c r="Q254">
         <v>0.26204290201678598</v>
       </c>
+      <c r="V254">
+        <v>857.1</v>
+      </c>
+      <c r="W254">
+        <f>330.6/2</f>
+        <v>165.3</v>
+      </c>
       <c r="Y254">
         <v>184.96333333333334</v>
       </c>
@@ -13418,7 +13506,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="255" spans="1:38">
+    <row r="255" spans="1:38" hidden="1">
       <c r="A255" t="s">
         <v>14</v>
       </c>
@@ -13499,7 +13587,7 @@
         <v>5.3666666666666671</v>
       </c>
     </row>
-    <row r="256" spans="1:38">
+    <row r="256" spans="1:38" hidden="1">
       <c r="A256" t="s">
         <v>14</v>
       </c>
@@ -13588,7 +13676,7 @@
         <v>5.5500000000000007</v>
       </c>
     </row>
-    <row r="257" spans="1:38">
+    <row r="257" spans="1:38" hidden="1">
       <c r="A257" t="s">
         <v>14</v>
       </c>
@@ -13715,6 +13803,13 @@
       <c r="Q258">
         <v>0.23887717611423617</v>
       </c>
+      <c r="V258">
+        <v>792.7</v>
+      </c>
+      <c r="W258">
+        <f>51/2</f>
+        <v>25.5</v>
+      </c>
       <c r="Y258">
         <v>226.27875000000003</v>
       </c>
@@ -13750,7 +13845,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="259" spans="1:38">
+    <row r="259" spans="1:38" hidden="1">
       <c r="A259" t="s">
         <v>14</v>
       </c>
@@ -13831,7 +13926,7 @@
         <v>7.3000000000000007</v>
       </c>
     </row>
-    <row r="260" spans="1:38">
+    <row r="260" spans="1:38" hidden="1">
       <c r="A260" t="s">
         <v>14</v>
       </c>
@@ -13920,7 +14015,7 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="261" spans="1:38">
+    <row r="261" spans="1:38" hidden="1">
       <c r="A261" t="s">
         <v>14</v>
       </c>
@@ -14047,6 +14142,13 @@
       <c r="Q262">
         <v>0.30976277716391826</v>
       </c>
+      <c r="V262">
+        <v>595</v>
+      </c>
+      <c r="W262">
+        <f>224/2</f>
+        <v>112</v>
+      </c>
       <c r="Y262">
         <v>181.26958333333334</v>
       </c>
@@ -14082,7 +14184,7 @@
         <v>14.59</v>
       </c>
     </row>
-    <row r="263" spans="1:38">
+    <row r="263" spans="1:38" hidden="1">
       <c r="A263" t="s">
         <v>14</v>
       </c>
@@ -14163,7 +14265,7 @@
         <v>5.4499999999999993</v>
       </c>
     </row>
-    <row r="264" spans="1:38">
+    <row r="264" spans="1:38" hidden="1">
       <c r="A264" t="s">
         <v>14</v>
       </c>
@@ -14252,7 +14354,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="265" spans="1:38">
+    <row r="265" spans="1:38" hidden="1">
       <c r="A265" t="s">
         <v>14</v>
       </c>
@@ -14379,6 +14481,13 @@
       <c r="Q266">
         <v>0.339017721945647</v>
       </c>
+      <c r="V266">
+        <v>642.5</v>
+      </c>
+      <c r="W266">
+        <f>305/2</f>
+        <v>152.5</v>
+      </c>
       <c r="Y266">
         <v>209.36958333333334</v>
       </c>
@@ -14414,7 +14523,7 @@
         <v>11.324999999999999</v>
       </c>
     </row>
-    <row r="267" spans="1:38">
+    <row r="267" spans="1:38" hidden="1">
       <c r="A267" t="s">
         <v>14</v>
       </c>
@@ -14495,7 +14604,7 @@
         <v>3.1500000000000004</v>
       </c>
     </row>
-    <row r="268" spans="1:38">
+    <row r="268" spans="1:38" hidden="1">
       <c r="A268" t="s">
         <v>14</v>
       </c>
@@ -14584,7 +14693,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="269" spans="1:38">
+    <row r="269" spans="1:38" hidden="1">
       <c r="A269" t="s">
         <v>14</v>
       </c>
@@ -14711,6 +14820,13 @@
       <c r="Q270">
         <v>0.18292425517668898</v>
       </c>
+      <c r="V270">
+        <v>863.1</v>
+      </c>
+      <c r="W270">
+        <f>412/2</f>
+        <v>206</v>
+      </c>
       <c r="Y270">
         <v>114.59750000000001</v>
       </c>
@@ -14746,7 +14862,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="271" spans="1:38">
+    <row r="271" spans="1:38" hidden="1">
       <c r="A271" t="s">
         <v>14</v>
       </c>
@@ -14827,7 +14943,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="272" spans="1:38">
+    <row r="272" spans="1:38" hidden="1">
       <c r="A272" t="s">
         <v>14</v>
       </c>
@@ -14916,7 +15032,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="273" spans="1:38">
+    <row r="273" spans="1:38" hidden="1">
       <c r="A273" t="s">
         <v>14</v>
       </c>
@@ -15043,6 +15159,13 @@
       <c r="Q274">
         <v>0.15193507160190126</v>
       </c>
+      <c r="V274">
+        <v>534.9</v>
+      </c>
+      <c r="W274">
+        <f>202/2</f>
+        <v>101</v>
+      </c>
       <c r="Y274">
         <v>123.38000000000001</v>
       </c>
@@ -15078,7 +15201,7 @@
         <v>13.8125</v>
       </c>
     </row>
-    <row r="275" spans="1:38">
+    <row r="275" spans="1:38" hidden="1">
       <c r="A275" t="s">
         <v>14</v>
       </c>
@@ -15159,7 +15282,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="276" spans="1:38">
+    <row r="276" spans="1:38" hidden="1">
       <c r="A276" t="s">
         <v>14</v>
       </c>
@@ -15248,7 +15371,7 @@
         <v>7.2000000000000011</v>
       </c>
     </row>
-    <row r="277" spans="1:38">
+    <row r="277" spans="1:38" hidden="1">
       <c r="A277" t="s">
         <v>14</v>
       </c>
@@ -15375,6 +15498,13 @@
       <c r="Q278">
         <v>0.25443084816614792</v>
       </c>
+      <c r="V278">
+        <v>839.6</v>
+      </c>
+      <c r="W278">
+        <f>410.4/2</f>
+        <v>205.2</v>
+      </c>
       <c r="Y278">
         <v>118.7325</v>
       </c>
@@ -15410,7 +15540,7 @@
         <v>11.15</v>
       </c>
     </row>
-    <row r="279" spans="1:38">
+    <row r="279" spans="1:38" hidden="1">
       <c r="A279" t="s">
         <v>14</v>
       </c>
@@ -15491,7 +15621,7 @@
         <v>2.7249999999999996</v>
       </c>
     </row>
-    <row r="280" spans="1:38">
+    <row r="280" spans="1:38" hidden="1">
       <c r="A280" t="s">
         <v>14</v>
       </c>
@@ -15580,7 +15710,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="281" spans="1:38">
+    <row r="281" spans="1:38" hidden="1">
       <c r="A281" t="s">
         <v>14</v>
       </c>
@@ -15707,6 +15837,13 @@
       <c r="Q282">
         <v>0.35198847194728033</v>
       </c>
+      <c r="V282">
+        <v>764.3</v>
+      </c>
+      <c r="W282">
+        <f>384.4/2</f>
+        <v>192.2</v>
+      </c>
       <c r="Y282">
         <v>101.39500000000001</v>
       </c>
@@ -15742,7 +15879,7 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="283" spans="1:38">
+    <row r="283" spans="1:38" hidden="1">
       <c r="A283" t="s">
         <v>14</v>
       </c>
@@ -15823,7 +15960,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="284" spans="1:38">
+    <row r="284" spans="1:38" hidden="1">
       <c r="A284" t="s">
         <v>14</v>
       </c>
@@ -15912,7 +16049,7 @@
         <v>7.375</v>
       </c>
     </row>
-    <row r="285" spans="1:38">
+    <row r="285" spans="1:38" hidden="1">
       <c r="A285" t="s">
         <v>14</v>
       </c>
@@ -16039,6 +16176,13 @@
       <c r="Q286">
         <v>0.21940645519328292</v>
       </c>
+      <c r="V286">
+        <v>626.5</v>
+      </c>
+      <c r="W286">
+        <f>213.5/2</f>
+        <v>106.75</v>
+      </c>
       <c r="Y286">
         <v>92.972499999999997</v>
       </c>
@@ -16074,7 +16218,7 @@
         <v>13.825000000000001</v>
       </c>
     </row>
-    <row r="287" spans="1:38">
+    <row r="287" spans="1:38" hidden="1">
       <c r="A287" t="s">
         <v>14</v>
       </c>
@@ -16155,7 +16299,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="288" spans="1:38">
+    <row r="288" spans="1:38" hidden="1">
       <c r="A288" t="s">
         <v>14</v>
       </c>
@@ -16244,7 +16388,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="289" spans="1:38">
+    <row r="289" spans="1:38" hidden="1">
       <c r="A289" t="s">
         <v>14</v>
       </c>
@@ -16371,6 +16515,13 @@
       <c r="Q290">
         <v>0.12858285098420077</v>
       </c>
+      <c r="V290">
+        <v>877.6</v>
+      </c>
+      <c r="W290">
+        <f>111.5/2</f>
+        <v>55.75</v>
+      </c>
       <c r="Y290">
         <v>152.08999999999997</v>
       </c>
@@ -16406,13 +16557,16 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="291" spans="1:38">
+    <row r="291" spans="1:38" hidden="1">
       <c r="A291" t="s">
         <v>14</v>
       </c>
       <c r="B291" t="s">
         <v>86</v>
       </c>
+      <c r="C291" s="7">
+        <v>44280</v>
+      </c>
       <c r="F291" t="s">
         <v>68</v>
       </c>
@@ -16450,13 +16604,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:38">
+    <row r="292" spans="1:38" hidden="1">
       <c r="A292" t="s">
         <v>14</v>
       </c>
       <c r="B292" t="s">
         <v>86</v>
       </c>
+      <c r="C292" s="7">
+        <v>44292</v>
+      </c>
       <c r="F292" t="s">
         <v>66</v>
       </c>
@@ -16494,13 +16651,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:38">
+    <row r="293" spans="1:38" hidden="1">
       <c r="A293" t="s">
         <v>14</v>
       </c>
       <c r="B293" t="s">
         <v>86</v>
       </c>
+      <c r="C293" s="7">
+        <v>44307</v>
+      </c>
       <c r="F293" t="s">
         <v>67</v>
       </c>
@@ -16538,13 +16698,16 @@
         <v>1.1159030349153662</v>
       </c>
     </row>
-    <row r="294" spans="1:38">
+    <row r="294" spans="1:38" hidden="1">
       <c r="A294" t="s">
         <v>14</v>
       </c>
       <c r="B294" t="s">
         <v>86</v>
       </c>
+      <c r="C294" s="7">
+        <v>44333</v>
+      </c>
       <c r="F294" t="s">
         <v>12</v>
       </c>
@@ -16575,6 +16738,13 @@
       <c r="Q294">
         <v>0.28430733360165567</v>
       </c>
+      <c r="V294">
+        <v>1819</v>
+      </c>
+      <c r="W294">
+        <f>87.4/2</f>
+        <v>43.7</v>
+      </c>
       <c r="Y294">
         <v>305.72749999999996</v>
       </c>
@@ -16582,13 +16752,16 @@
         <v>19.981315178185927</v>
       </c>
     </row>
-    <row r="295" spans="1:38">
+    <row r="295" spans="1:38" hidden="1">
       <c r="A295" t="s">
         <v>14</v>
       </c>
       <c r="B295" t="s">
         <v>87</v>
       </c>
+      <c r="C295" s="7">
+        <v>44280</v>
+      </c>
       <c r="F295" t="s">
         <v>68</v>
       </c>
@@ -16626,13 +16799,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:38">
+    <row r="296" spans="1:38" hidden="1">
       <c r="A296" t="s">
         <v>14</v>
       </c>
       <c r="B296" t="s">
         <v>87</v>
       </c>
+      <c r="C296" s="7">
+        <v>44292</v>
+      </c>
       <c r="F296" t="s">
         <v>66</v>
       </c>
@@ -16670,13 +16846,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:38">
+    <row r="297" spans="1:38" hidden="1">
       <c r="A297" t="s">
         <v>14</v>
       </c>
       <c r="B297" t="s">
         <v>87</v>
       </c>
+      <c r="C297" s="7">
+        <v>44307</v>
+      </c>
       <c r="F297" t="s">
         <v>67</v>
       </c>
@@ -16721,6 +16900,9 @@
       <c r="B298" t="s">
         <v>87</v>
       </c>
+      <c r="C298" s="7">
+        <v>44336</v>
+      </c>
       <c r="F298" t="s">
         <v>12</v>
       </c>
@@ -16751,6 +16933,13 @@
       <c r="Q298">
         <v>0.13443861621855505</v>
       </c>
+      <c r="V298">
+        <v>1488</v>
+      </c>
+      <c r="W298">
+        <f>275/2</f>
+        <v>137.5</v>
+      </c>
       <c r="Y298">
         <v>238.78749999999999</v>
       </c>
@@ -16758,13 +16947,16 @@
         <v>25.523318908438497</v>
       </c>
     </row>
-    <row r="299" spans="1:38">
+    <row r="299" spans="1:38" hidden="1">
       <c r="A299" t="s">
         <v>14</v>
       </c>
       <c r="B299" t="s">
         <v>88</v>
       </c>
+      <c r="C299" s="7">
+        <v>44280</v>
+      </c>
       <c r="F299" t="s">
         <v>68</v>
       </c>
@@ -16802,13 +16994,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:38">
+    <row r="300" spans="1:38" hidden="1">
       <c r="A300" t="s">
         <v>14</v>
       </c>
       <c r="B300" t="s">
         <v>88</v>
       </c>
+      <c r="C300" s="7">
+        <v>44292</v>
+      </c>
       <c r="F300" t="s">
         <v>66</v>
       </c>
@@ -16846,13 +17041,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:38">
+    <row r="301" spans="1:38" hidden="1">
       <c r="A301" t="s">
         <v>14</v>
       </c>
       <c r="B301" t="s">
         <v>88</v>
       </c>
+      <c r="C301" s="7">
+        <v>44309</v>
+      </c>
       <c r="F301" t="s">
         <v>67</v>
       </c>
@@ -16897,6 +17095,9 @@
       <c r="B302" t="s">
         <v>88</v>
       </c>
+      <c r="C302" s="7">
+        <v>44340</v>
+      </c>
       <c r="F302" t="s">
         <v>12</v>
       </c>
@@ -16927,6 +17128,13 @@
       <c r="Q302">
         <v>0.21671755749592439</v>
       </c>
+      <c r="V302">
+        <v>1678</v>
+      </c>
+      <c r="W302">
+        <f>287.6/2</f>
+        <v>143.80000000000001</v>
+      </c>
       <c r="Y302">
         <v>247.53625</v>
       </c>
@@ -16934,13 +17142,16 @@
         <v>5.2749446361410799</v>
       </c>
     </row>
-    <row r="303" spans="1:38">
+    <row r="303" spans="1:38" hidden="1">
       <c r="A303" t="s">
         <v>14</v>
       </c>
       <c r="B303" t="s">
         <v>89</v>
       </c>
+      <c r="C303" s="7">
+        <v>44280</v>
+      </c>
       <c r="F303" t="s">
         <v>68</v>
       </c>
@@ -16978,13 +17189,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:38">
+    <row r="304" spans="1:38" hidden="1">
       <c r="A304" t="s">
         <v>14</v>
       </c>
       <c r="B304" t="s">
         <v>89</v>
       </c>
+      <c r="C304" s="7">
+        <v>44292</v>
+      </c>
       <c r="F304" t="s">
         <v>66</v>
       </c>
@@ -17022,13 +17236,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:26">
+    <row r="305" spans="1:26" hidden="1">
       <c r="A305" t="s">
         <v>14</v>
       </c>
       <c r="B305" t="s">
         <v>89</v>
       </c>
+      <c r="C305" s="7">
+        <v>44309</v>
+      </c>
       <c r="F305" t="s">
         <v>67</v>
       </c>
@@ -17073,6 +17290,9 @@
       <c r="B306" t="s">
         <v>89</v>
       </c>
+      <c r="C306" s="7">
+        <v>44336</v>
+      </c>
       <c r="F306" t="s">
         <v>12</v>
       </c>
@@ -17103,6 +17323,13 @@
       <c r="Q306">
         <v>0.25217879221598083</v>
       </c>
+      <c r="V306">
+        <v>1347</v>
+      </c>
+      <c r="W306">
+        <f>289/2</f>
+        <v>144.5</v>
+      </c>
       <c r="Y306">
         <v>251.11666666666662</v>
       </c>
@@ -17110,13 +17337,16 @@
         <v>30.747951121142297</v>
       </c>
     </row>
-    <row r="307" spans="1:26">
+    <row r="307" spans="1:26" hidden="1">
       <c r="A307" t="s">
         <v>14</v>
       </c>
       <c r="B307" t="s">
         <v>90</v>
       </c>
+      <c r="C307" s="7">
+        <v>44280</v>
+      </c>
       <c r="F307" t="s">
         <v>68</v>
       </c>
@@ -17154,13 +17384,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:26">
+    <row r="308" spans="1:26" hidden="1">
       <c r="A308" t="s">
         <v>14</v>
       </c>
       <c r="B308" t="s">
         <v>90</v>
       </c>
+      <c r="C308" s="7">
+        <v>44292</v>
+      </c>
       <c r="F308" t="s">
         <v>66</v>
       </c>
@@ -17198,13 +17431,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:26">
+    <row r="309" spans="1:26" hidden="1">
       <c r="A309" t="s">
         <v>14</v>
       </c>
       <c r="B309" t="s">
         <v>90</v>
       </c>
+      <c r="C309" s="7">
+        <v>44316</v>
+      </c>
       <c r="F309" t="s">
         <v>67</v>
       </c>
@@ -17249,6 +17485,9 @@
       <c r="B310" t="s">
         <v>90</v>
       </c>
+      <c r="C310" s="7">
+        <v>44340</v>
+      </c>
       <c r="F310" t="s">
         <v>12</v>
       </c>
@@ -17279,6 +17518,13 @@
       <c r="Q310">
         <v>0.46930046610728415</v>
       </c>
+      <c r="V310">
+        <v>1111</v>
+      </c>
+      <c r="W310">
+        <f>307.2/2</f>
+        <v>153.6</v>
+      </c>
       <c r="Y310">
         <v>193.07416666666668</v>
       </c>
@@ -17286,13 +17532,16 @@
         <v>25.765741920483489</v>
       </c>
     </row>
-    <row r="311" spans="1:26">
+    <row r="311" spans="1:26" hidden="1">
       <c r="A311" t="s">
         <v>14</v>
       </c>
       <c r="B311" t="s">
         <v>91</v>
       </c>
+      <c r="C311" s="7">
+        <v>44280</v>
+      </c>
       <c r="F311" t="s">
         <v>68</v>
       </c>
@@ -17330,13 +17579,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:26">
+    <row r="312" spans="1:26" hidden="1">
       <c r="A312" t="s">
         <v>14</v>
       </c>
       <c r="B312" t="s">
         <v>91</v>
       </c>
+      <c r="C312" s="7">
+        <v>44292</v>
+      </c>
       <c r="F312" t="s">
         <v>66</v>
       </c>
@@ -17374,13 +17626,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:26">
+    <row r="313" spans="1:26" hidden="1">
       <c r="A313" t="s">
         <v>14</v>
       </c>
       <c r="B313" t="s">
         <v>91</v>
       </c>
+      <c r="C313" s="7">
+        <v>44309</v>
+      </c>
       <c r="F313" t="s">
         <v>67</v>
       </c>
@@ -17425,6 +17680,9 @@
       <c r="B314" t="s">
         <v>91</v>
       </c>
+      <c r="C314" s="7">
+        <v>44340</v>
+      </c>
       <c r="F314" t="s">
         <v>12</v>
       </c>
@@ -17455,6 +17713,13 @@
       <c r="Q314">
         <v>0.37863698360559983</v>
       </c>
+      <c r="V314">
+        <v>1157</v>
+      </c>
+      <c r="W314">
+        <f>255.3/2</f>
+        <v>127.65</v>
+      </c>
       <c r="Y314">
         <v>181.91583333333332</v>
       </c>
@@ -17462,13 +17727,16 @@
         <v>21.196272061510136</v>
       </c>
     </row>
-    <row r="315" spans="1:26">
+    <row r="315" spans="1:26" hidden="1">
       <c r="A315" t="s">
         <v>14</v>
       </c>
       <c r="B315" t="s">
         <v>92</v>
       </c>
+      <c r="C315" s="7">
+        <v>44242</v>
+      </c>
       <c r="F315" t="s">
         <v>68</v>
       </c>
@@ -17506,13 +17774,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:26">
+    <row r="316" spans="1:26" hidden="1">
       <c r="A316" t="s">
         <v>14</v>
       </c>
       <c r="B316" t="s">
         <v>92</v>
       </c>
+      <c r="C316" s="7">
+        <v>44250</v>
+      </c>
       <c r="F316" t="s">
         <v>66</v>
       </c>
@@ -17550,13 +17821,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:26">
+    <row r="317" spans="1:26" hidden="1">
       <c r="A317" t="s">
         <v>14</v>
       </c>
       <c r="B317" t="s">
         <v>92</v>
       </c>
+      <c r="C317" s="7">
+        <v>44263</v>
+      </c>
       <c r="F317" t="s">
         <v>67</v>
       </c>
@@ -17601,6 +17875,9 @@
       <c r="B318" t="s">
         <v>92</v>
       </c>
+      <c r="C318" s="7">
+        <v>44281</v>
+      </c>
       <c r="F318" t="s">
         <v>12</v>
       </c>
@@ -17631,6 +17908,13 @@
       <c r="Q318">
         <v>0.20885329505485128</v>
       </c>
+      <c r="V318">
+        <v>1503</v>
+      </c>
+      <c r="W318">
+        <f>383/2</f>
+        <v>191.5</v>
+      </c>
       <c r="Y318">
         <v>168.46416666666667</v>
       </c>
@@ -17638,13 +17922,16 @@
         <v>15.757838400771089</v>
       </c>
     </row>
-    <row r="319" spans="1:26">
+    <row r="319" spans="1:26" hidden="1">
       <c r="A319" t="s">
         <v>14</v>
       </c>
       <c r="B319" t="s">
         <v>93</v>
       </c>
+      <c r="C319" s="7">
+        <v>44242</v>
+      </c>
       <c r="F319" t="s">
         <v>68</v>
       </c>
@@ -17682,13 +17969,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:26">
+    <row r="320" spans="1:26" hidden="1">
       <c r="A320" t="s">
         <v>14</v>
       </c>
       <c r="B320" t="s">
         <v>93</v>
       </c>
+      <c r="C320" s="7">
+        <v>44250</v>
+      </c>
       <c r="F320" t="s">
         <v>66</v>
       </c>
@@ -17726,13 +18016,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:26">
+    <row r="321" spans="1:26" hidden="1">
       <c r="A321" t="s">
         <v>14</v>
       </c>
       <c r="B321" t="s">
         <v>93</v>
       </c>
+      <c r="C321" s="7">
+        <v>44259</v>
+      </c>
       <c r="F321" t="s">
         <v>67</v>
       </c>
@@ -17777,6 +18070,9 @@
       <c r="B322" t="s">
         <v>93</v>
       </c>
+      <c r="C322" s="7">
+        <v>44281</v>
+      </c>
       <c r="F322" t="s">
         <v>12</v>
       </c>
@@ -17807,6 +18103,13 @@
       <c r="Q322">
         <v>0.285520293521349</v>
       </c>
+      <c r="V322">
+        <v>1575</v>
+      </c>
+      <c r="W322">
+        <f>366/2</f>
+        <v>183</v>
+      </c>
       <c r="Y322">
         <v>156.185</v>
       </c>
@@ -17814,13 +18117,16 @@
         <v>29.401922981328966</v>
       </c>
     </row>
-    <row r="323" spans="1:26">
+    <row r="323" spans="1:26" hidden="1">
       <c r="A323" t="s">
         <v>14</v>
       </c>
       <c r="B323" t="s">
         <v>94</v>
       </c>
+      <c r="C323" s="7">
+        <v>44242</v>
+      </c>
       <c r="F323" t="s">
         <v>68</v>
       </c>
@@ -17858,13 +18164,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:26">
+    <row r="324" spans="1:26" hidden="1">
       <c r="A324" t="s">
         <v>14</v>
       </c>
       <c r="B324" t="s">
         <v>94</v>
       </c>
+      <c r="C324" s="7">
+        <v>44250</v>
+      </c>
       <c r="F324" t="s">
         <v>66</v>
       </c>
@@ -17902,13 +18211,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:26">
+    <row r="325" spans="1:26" hidden="1">
       <c r="A325" t="s">
         <v>14</v>
       </c>
       <c r="B325" t="s">
         <v>94</v>
       </c>
+      <c r="C325" s="7">
+        <v>44264</v>
+      </c>
       <c r="F325" t="s">
         <v>67</v>
       </c>
@@ -17953,6 +18265,9 @@
       <c r="B326" t="s">
         <v>94</v>
       </c>
+      <c r="C326" s="7">
+        <v>44286</v>
+      </c>
       <c r="F326" t="s">
         <v>12</v>
       </c>
@@ -17983,6 +18298,13 @@
       <c r="Q326">
         <v>0.34833275077169285</v>
       </c>
+      <c r="V326">
+        <v>1597</v>
+      </c>
+      <c r="W326">
+        <f>362/2</f>
+        <v>181</v>
+      </c>
       <c r="Y326">
         <v>192.4375</v>
       </c>
@@ -17990,13 +18312,16 @@
         <v>50.899819059836311</v>
       </c>
     </row>
-    <row r="327" spans="1:26">
+    <row r="327" spans="1:26" hidden="1">
       <c r="A327" t="s">
         <v>14</v>
       </c>
       <c r="B327" t="s">
         <v>95</v>
       </c>
+      <c r="C327" s="7">
+        <v>44242</v>
+      </c>
       <c r="F327" t="s">
         <v>68</v>
       </c>
@@ -18034,13 +18359,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:26">
+    <row r="328" spans="1:26" hidden="1">
       <c r="A328" t="s">
         <v>14</v>
       </c>
       <c r="B328" t="s">
         <v>95</v>
       </c>
+      <c r="C328" s="7">
+        <v>44250</v>
+      </c>
       <c r="F328" t="s">
         <v>66</v>
       </c>
@@ -18078,13 +18406,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:26">
+    <row r="329" spans="1:26" hidden="1">
       <c r="A329" t="s">
         <v>14</v>
       </c>
       <c r="B329" t="s">
         <v>95</v>
       </c>
+      <c r="C329" s="7">
+        <v>44264</v>
+      </c>
       <c r="F329" t="s">
         <v>67</v>
       </c>
@@ -18129,6 +18460,9 @@
       <c r="B330" t="s">
         <v>95</v>
       </c>
+      <c r="C330" s="7">
+        <v>44286</v>
+      </c>
       <c r="F330" t="s">
         <v>12</v>
       </c>
@@ -18159,6 +18493,13 @@
       <c r="Q330">
         <v>0.76296336507168472</v>
       </c>
+      <c r="V330">
+        <v>1534</v>
+      </c>
+      <c r="W330">
+        <f>442.4/2</f>
+        <v>221.2</v>
+      </c>
       <c r="Y330">
         <v>203.17</v>
       </c>
@@ -18166,13 +18507,16 @@
         <v>24.558059135821743</v>
       </c>
     </row>
-    <row r="331" spans="1:26">
+    <row r="331" spans="1:26" hidden="1">
       <c r="A331" t="s">
         <v>14</v>
       </c>
       <c r="B331" t="s">
         <v>96</v>
       </c>
+      <c r="C331" s="7">
+        <v>44242</v>
+      </c>
       <c r="F331" t="s">
         <v>68</v>
       </c>
@@ -18210,13 +18554,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:26">
+    <row r="332" spans="1:26" hidden="1">
       <c r="A332" t="s">
         <v>14</v>
       </c>
       <c r="B332" t="s">
         <v>96</v>
       </c>
+      <c r="C332" s="7">
+        <v>44250</v>
+      </c>
       <c r="F332" t="s">
         <v>66</v>
       </c>
@@ -18254,13 +18601,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:26">
+    <row r="333" spans="1:26" hidden="1">
       <c r="A333" t="s">
         <v>14</v>
       </c>
       <c r="B333" t="s">
         <v>96</v>
       </c>
+      <c r="C333" s="7">
+        <v>44263</v>
+      </c>
       <c r="F333" t="s">
         <v>67</v>
       </c>
@@ -18305,6 +18655,9 @@
       <c r="B334" t="s">
         <v>96</v>
       </c>
+      <c r="C334" s="7">
+        <v>44286</v>
+      </c>
       <c r="F334" t="s">
         <v>12</v>
       </c>
@@ -18335,6 +18688,13 @@
       <c r="Q334">
         <v>0.10615321442144372</v>
       </c>
+      <c r="V334">
+        <v>781</v>
+      </c>
+      <c r="W334">
+        <f>244/2</f>
+        <v>122</v>
+      </c>
       <c r="Y334">
         <v>191.30291666666665</v>
       </c>
@@ -18342,13 +18702,16 @@
         <v>42.470371984124505</v>
       </c>
     </row>
-    <row r="335" spans="1:26">
+    <row r="335" spans="1:26" hidden="1">
       <c r="A335" t="s">
         <v>14</v>
       </c>
       <c r="B335" t="s">
         <v>97</v>
       </c>
+      <c r="C335" s="7">
+        <v>44242</v>
+      </c>
       <c r="F335" t="s">
         <v>68</v>
       </c>
@@ -18386,13 +18749,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:26">
+    <row r="336" spans="1:26" hidden="1">
       <c r="A336" t="s">
         <v>14</v>
       </c>
       <c r="B336" t="s">
         <v>97</v>
       </c>
+      <c r="C336" s="7">
+        <v>44250</v>
+      </c>
       <c r="F336" t="s">
         <v>66</v>
       </c>
@@ -18430,13 +18796,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:26">
+    <row r="337" spans="1:26" hidden="1">
       <c r="A337" t="s">
         <v>14</v>
       </c>
       <c r="B337" t="s">
         <v>97</v>
       </c>
+      <c r="C337" s="7">
+        <v>44263</v>
+      </c>
       <c r="F337" t="s">
         <v>67</v>
       </c>
@@ -18481,6 +18850,9 @@
       <c r="B338" t="s">
         <v>97</v>
       </c>
+      <c r="C338" s="7">
+        <v>44286</v>
+      </c>
       <c r="F338" t="s">
         <v>12</v>
       </c>
@@ -18511,6 +18883,13 @@
       <c r="Q338">
         <v>0.43671030023484692</v>
       </c>
+      <c r="V338">
+        <v>1665</v>
+      </c>
+      <c r="W338">
+        <f>464.4/2</f>
+        <v>232.2</v>
+      </c>
       <c r="Y338">
         <v>195.16291666666669</v>
       </c>
@@ -18519,10 +18898,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL338" xr:uid="{82E1BEE1-02EA-47DB-B89F-8184F465ECFF}">
+  <autoFilter ref="A1:AL338" xr:uid="{D9F824F1-C9CA-4B4A-8D6A-E1D6F0626745}">
     <filterColumn colId="1">
       <filters>
-        <filter val="TOSyear3SowFeb21CvBerken"/>
         <filter val="TOSyear3SowFeb21CvCeleraII"/>
         <filter val="TOSyear3SowFeb21CvCrystal"/>
         <filter val="TOSyear3SowFeb21CvJade"/>
@@ -18554,6 +18932,11 @@
         <filter val="TOSyear3SowSept20CvOpal"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="HarvestRipe"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AL290">
     <sortCondition ref="B2:B290"/>

</xml_diff>

<commit_message>
Checked TOS data and updated dataset in model
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/TOSobserved.xlsx
+++ b/Prototypes/Mungbean/TOSobserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD3CC35-374F-4161-9E36-CC23DBAE45EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70466632-B26E-47B2-8937-BC43C3E10725}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01D3E681-48EE-4304-AF98-4E94EBE61D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -856,12 +856,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3519DD51-BED6-4262-8A50-4DB48CCAF26B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AL338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V298" sqref="V298"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -989,7 +988,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:38" hidden="1">
+    <row r="2" spans="1:38">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>57.25</v>
       </c>
     </row>
-    <row r="3" spans="1:38" hidden="1">
+    <row r="3" spans="1:38">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1157,7 @@
         <v>57.25</v>
       </c>
     </row>
-    <row r="4" spans="1:38" hidden="1">
+    <row r="4" spans="1:38">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1179,7 +1178,7 @@
       </c>
       <c r="AC4" s="15"/>
     </row>
-    <row r="5" spans="1:38" hidden="1">
+    <row r="5" spans="1:38">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:38" hidden="1">
+    <row r="6" spans="1:38">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1345,7 +1344,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:38" hidden="1">
+    <row r="7" spans="1:38">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1366,7 +1365,7 @@
       </c>
       <c r="AC7" s="15"/>
     </row>
-    <row r="8" spans="1:38" hidden="1">
+    <row r="8" spans="1:38">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1387,7 +1386,7 @@
       </c>
       <c r="AC8" s="15"/>
     </row>
-    <row r="9" spans="1:38" hidden="1">
+    <row r="9" spans="1:38">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1459,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:38" hidden="1">
+    <row r="10" spans="1:38">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1480,7 @@
       </c>
       <c r="AC10" s="15"/>
     </row>
-    <row r="11" spans="1:38" hidden="1">
+    <row r="11" spans="1:38">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1502,7 +1501,7 @@
       </c>
       <c r="AC11" s="15"/>
     </row>
-    <row r="12" spans="1:38" hidden="1">
+    <row r="12" spans="1:38">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1523,7 +1522,7 @@
       </c>
       <c r="AC12" s="15"/>
     </row>
-    <row r="13" spans="1:38" hidden="1">
+    <row r="13" spans="1:38">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1617,7 +1616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:38" hidden="1">
+    <row r="14" spans="1:38">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1637,7 @@
       </c>
       <c r="AC14" s="15"/>
     </row>
-    <row r="15" spans="1:38" hidden="1">
+    <row r="15" spans="1:38">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +1708,7 @@
         <v>76.25</v>
       </c>
     </row>
-    <row r="16" spans="1:38" hidden="1">
+    <row r="16" spans="1:38">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1730,7 +1729,7 @@
       </c>
       <c r="AC16" s="15"/>
     </row>
-    <row r="17" spans="1:38" hidden="1">
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1751,7 +1750,7 @@
       </c>
       <c r="AC17" s="15"/>
     </row>
-    <row r="18" spans="1:38" s="9" customFormat="1" hidden="1">
+    <row r="18" spans="1:38" s="9" customFormat="1">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1803,7 +1802,7 @@
       <c r="AK18"/>
       <c r="AL18"/>
     </row>
-    <row r="19" spans="1:38" s="9" customFormat="1" hidden="1">
+    <row r="19" spans="1:38" s="9" customFormat="1">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1903,7 +1902,7 @@
       <c r="AK19"/>
       <c r="AL19"/>
     </row>
-    <row r="20" spans="1:38" s="9" customFormat="1" hidden="1">
+    <row r="20" spans="1:38" s="9" customFormat="1">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1993,7 +1992,7 @@
       <c r="AK20"/>
       <c r="AL20"/>
     </row>
-    <row r="21" spans="1:38" s="9" customFormat="1" hidden="1">
+    <row r="21" spans="1:38" s="9" customFormat="1">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2043,7 @@
       <c r="AK21"/>
       <c r="AL21"/>
     </row>
-    <row r="22" spans="1:38" hidden="1">
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2065,7 +2064,7 @@
       </c>
       <c r="AC22" s="15"/>
     </row>
-    <row r="23" spans="1:38" hidden="1">
+    <row r="23" spans="1:38">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="24" spans="1:38" hidden="1">
+    <row r="24" spans="1:38">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -2180,7 +2179,7 @@
       </c>
       <c r="AC24" s="15"/>
     </row>
-    <row r="25" spans="1:38" hidden="1">
+    <row r="25" spans="1:38">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>55.75</v>
       </c>
     </row>
-    <row r="26" spans="1:38" hidden="1">
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2277,7 +2276,7 @@
       </c>
       <c r="AC26" s="15"/>
     </row>
-    <row r="27" spans="1:38" hidden="1">
+    <row r="27" spans="1:38">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2298,7 +2297,7 @@
       </c>
       <c r="AC27" s="15"/>
     </row>
-    <row r="28" spans="1:38" hidden="1">
+    <row r="28" spans="1:38">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>55.75</v>
       </c>
     </row>
-    <row r="29" spans="1:38" hidden="1">
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2413,7 +2412,7 @@
       </c>
       <c r="AC29" s="15"/>
     </row>
-    <row r="30" spans="1:38" hidden="1">
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2436,7 +2435,7 @@
         <v>7.6933309835944632</v>
       </c>
     </row>
-    <row r="31" spans="1:38" hidden="1">
+    <row r="31" spans="1:38">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>1.2063290642635434</v>
       </c>
     </row>
-    <row r="32" spans="1:38" hidden="1">
+    <row r="32" spans="1:38">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2536,7 +2535,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="33" spans="1:38" hidden="1">
+    <row r="33" spans="1:38">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2559,7 +2558,7 @@
         <v>4.7694179276883206</v>
       </c>
     </row>
-    <row r="34" spans="1:38" hidden="1">
+    <row r="34" spans="1:38">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="35" spans="1:38" hidden="1">
+    <row r="35" spans="1:38">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>95.562706876684871</v>
       </c>
     </row>
-    <row r="36" spans="1:38" hidden="1">
+    <row r="36" spans="1:38">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2745,7 +2744,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="37" spans="1:38" hidden="1">
+    <row r="37" spans="1:38">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>85.365260888374024</v>
       </c>
     </row>
-    <row r="38" spans="1:38" hidden="1">
+    <row r="38" spans="1:38">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2785,7 +2784,7 @@
         <v>78.19911730793919</v>
       </c>
     </row>
-    <row r="39" spans="1:38" hidden="1">
+    <row r="39" spans="1:38">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2820,7 +2819,7 @@
         <v>51.166571443993753</v>
       </c>
       <c r="N39">
-        <v>709.34</v>
+        <v>704.08749999999986</v>
       </c>
       <c r="O39">
         <v>40.440228527214089</v>
@@ -2886,7 +2885,7 @@
         <v>11.049999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:38" hidden="1">
+    <row r="40" spans="1:38">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2963,7 +2962,7 @@
         <v>5.7499999999999991</v>
       </c>
     </row>
-    <row r="41" spans="1:38" hidden="1">
+    <row r="41" spans="1:38">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>7.0500000000000007</v>
       </c>
     </row>
-    <row r="42" spans="1:38" hidden="1">
+    <row r="42" spans="1:38">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="43" spans="1:38" hidden="1">
+    <row r="43" spans="1:38">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -3164,7 +3163,7 @@
         <v>26.413876403638049</v>
       </c>
       <c r="N43">
-        <v>472.48</v>
+        <v>460.1875</v>
       </c>
       <c r="O43">
         <v>45.603571314828621</v>
@@ -3230,7 +3229,7 @@
         <v>10.100000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:38" hidden="1">
+    <row r="44" spans="1:38">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>1.9550267916612909</v>
       </c>
     </row>
-    <row r="45" spans="1:38" hidden="1">
+    <row r="45" spans="1:38">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -3276,7 +3275,7 @@
         <v>7.0887136859119897</v>
       </c>
     </row>
-    <row r="46" spans="1:38" hidden="1">
+    <row r="46" spans="1:38">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -3353,7 +3352,7 @@
         <v>3.4499999999999993</v>
       </c>
     </row>
-    <row r="47" spans="1:38" hidden="1">
+    <row r="47" spans="1:38">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3436,7 +3435,7 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="48" spans="1:38" hidden="1">
+    <row r="48" spans="1:38">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -3459,7 +3458,7 @@
         <v>6.5364891596497223</v>
       </c>
     </row>
-    <row r="49" spans="1:38" hidden="1">
+    <row r="49" spans="1:38">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -3542,7 +3541,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="50" spans="1:38" hidden="1">
+    <row r="50" spans="1:38">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3562,7 +3561,7 @@
         <v>78.664427905902855</v>
       </c>
     </row>
-    <row r="51" spans="1:38" hidden="1">
+    <row r="51" spans="1:38">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -3582,7 +3581,7 @@
         <v>69.378993307278549</v>
       </c>
     </row>
-    <row r="52" spans="1:38" hidden="1">
+    <row r="52" spans="1:38">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -3683,7 +3682,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="53" spans="1:38" hidden="1">
+    <row r="53" spans="1:38">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>60.228081113641714</v>
       </c>
     </row>
-    <row r="54" spans="1:38" hidden="1">
+    <row r="54" spans="1:38">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3726,7 +3725,7 @@
         <v>6.9378865308974476</v>
       </c>
     </row>
-    <row r="55" spans="1:38" hidden="1">
+    <row r="55" spans="1:38">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>5.7038091949066416</v>
       </c>
     </row>
-    <row r="56" spans="1:38" hidden="1">
+    <row r="56" spans="1:38">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -3826,7 +3825,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="57" spans="1:38" hidden="1">
+    <row r="57" spans="1:38">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3849,7 +3848,7 @@
         <v>4.1501234511883522</v>
       </c>
     </row>
-    <row r="58" spans="1:38" hidden="1">
+    <row r="58" spans="1:38">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>7.15</v>
       </c>
     </row>
-    <row r="59" spans="1:38" hidden="1">
+    <row r="59" spans="1:38">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>80.862721056211299</v>
       </c>
     </row>
-    <row r="60" spans="1:38" hidden="1">
+    <row r="60" spans="1:38">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -4029,7 +4028,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="61" spans="1:38" hidden="1">
+    <row r="61" spans="1:38">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -4049,7 +4048,7 @@
         <v>76.649769492121663</v>
       </c>
     </row>
-    <row r="62" spans="1:38" hidden="1">
+    <row r="62" spans="1:38">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -4069,7 +4068,7 @@
         <v>63.163184444804152</v>
       </c>
     </row>
-    <row r="63" spans="1:38" hidden="1">
+    <row r="63" spans="1:38">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -4098,7 +4097,7 @@
         <v>25.863853275372517</v>
       </c>
       <c r="N63">
-        <v>650.82749999999999</v>
+        <v>644.96499999999992</v>
       </c>
       <c r="O63">
         <v>93.626634509541802</v>
@@ -4164,7 +4163,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="64" spans="1:38" hidden="1">
+    <row r="64" spans="1:38">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>0.88569363214705221</v>
       </c>
     </row>
-    <row r="65" spans="1:38" hidden="1">
+    <row r="65" spans="1:38">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -4210,7 +4209,7 @@
         <v>3.7460992507946012</v>
       </c>
     </row>
-    <row r="66" spans="1:38" hidden="1">
+    <row r="66" spans="1:38">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>5.1999999999999993</v>
       </c>
     </row>
-    <row r="67" spans="1:38" hidden="1">
+    <row r="67" spans="1:38">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -4370,7 +4369,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="68" spans="1:38" hidden="1">
+    <row r="68" spans="1:38">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -4393,7 +4392,7 @@
         <v>7.2406411781241697</v>
       </c>
     </row>
-    <row r="69" spans="1:38" hidden="1">
+    <row r="69" spans="1:38">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="70" spans="1:38" hidden="1">
+    <row r="70" spans="1:38">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>5.184676906749023</v>
       </c>
     </row>
-    <row r="71" spans="1:38" hidden="1">
+    <row r="71" spans="1:38">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4516,7 +4515,7 @@
         <v>7.8407817163666476</v>
       </c>
     </row>
-    <row r="72" spans="1:38" hidden="1">
+    <row r="72" spans="1:38">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4551,7 +4550,7 @@
         <v>8.2773526363607672</v>
       </c>
       <c r="N72">
-        <v>391.90250000000003</v>
+        <v>383.88</v>
       </c>
       <c r="O72">
         <v>48.786462325628719</v>
@@ -4617,7 +4616,7 @@
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:38" hidden="1">
+    <row r="73" spans="1:38">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4640,7 +4639,7 @@
         <v>6.7197832300470814</v>
       </c>
     </row>
-    <row r="74" spans="1:38" hidden="1">
+    <row r="74" spans="1:38">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>3.0064167947143599</v>
       </c>
     </row>
-    <row r="75" spans="1:38" hidden="1">
+    <row r="75" spans="1:38">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>5.7397344050545707</v>
       </c>
     </row>
-    <row r="76" spans="1:38" hidden="1">
+    <row r="76" spans="1:38">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4709,7 +4708,7 @@
         <v>7.452611027121165</v>
       </c>
     </row>
-    <row r="77" spans="1:38" hidden="1">
+    <row r="77" spans="1:38">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4732,7 +4731,7 @@
         <v>4.8461663877908547</v>
       </c>
     </row>
-    <row r="78" spans="1:38" hidden="1">
+    <row r="78" spans="1:38">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>4.6436072571595615</v>
       </c>
     </row>
-    <row r="79" spans="1:38" hidden="1">
+    <row r="79" spans="1:38">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4778,7 +4777,7 @@
         <v>5.8083684708497749</v>
       </c>
     </row>
-    <row r="80" spans="1:38" hidden="1">
+    <row r="80" spans="1:38">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4801,7 +4800,7 @@
         <v>6.4887549172994783</v>
       </c>
     </row>
-    <row r="81" spans="1:38" hidden="1">
+    <row r="81" spans="1:38">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4824,7 +4823,7 @@
         <v>6.2852775311886555</v>
       </c>
     </row>
-    <row r="82" spans="1:38" hidden="1">
+    <row r="82" spans="1:38">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4901,7 +4900,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="83" spans="1:38" hidden="1">
+    <row r="83" spans="1:38">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4924,7 +4923,7 @@
         <v>3.1010758048730089</v>
       </c>
     </row>
-    <row r="84" spans="1:38" hidden="1">
+    <row r="84" spans="1:38">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -5013,7 +5012,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="85" spans="1:38" hidden="1">
+    <row r="85" spans="1:38">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -5036,7 +5035,7 @@
         <v>1.5598329392157901</v>
       </c>
     </row>
-    <row r="86" spans="1:38" hidden="1">
+    <row r="86" spans="1:38">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="87" spans="1:38" hidden="1">
+    <row r="87" spans="1:38">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -5140,7 +5139,7 @@
         <v>4.4663725803537604</v>
       </c>
     </row>
-    <row r="88" spans="1:38" hidden="1">
+    <row r="88" spans="1:38">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>2.1212592634152689</v>
       </c>
     </row>
-    <row r="89" spans="1:38" hidden="1">
+    <row r="89" spans="1:38">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -5192,7 +5191,7 @@
         <v>14.720511412651387</v>
       </c>
       <c r="N89">
-        <v>439.23750000000001</v>
+        <v>429.61250000000001</v>
       </c>
       <c r="O89">
         <v>32.153378872470945</v>
@@ -5262,7 +5261,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="90" spans="1:38" hidden="1">
+    <row r="90" spans="1:38">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -5297,7 +5296,7 @@
         <v>6.9759324346881195</v>
       </c>
       <c r="N90">
-        <v>77.09</v>
+        <v>45.574999999999996</v>
       </c>
       <c r="O90">
         <v>9.3602332592017259</v>
@@ -5327,7 +5326,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:38" hidden="1">
+    <row r="91" spans="1:38">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -5350,7 +5349,7 @@
         <v>8.3177240795154255</v>
       </c>
     </row>
-    <row r="92" spans="1:38" hidden="1">
+    <row r="92" spans="1:38">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -5373,7 +5372,7 @@
         <v>2.2174056536026931</v>
       </c>
     </row>
-    <row r="93" spans="1:38" hidden="1">
+    <row r="93" spans="1:38">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -5446,7 +5445,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="94" spans="1:38" hidden="1">
+    <row r="94" spans="1:38">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -5466,7 +5465,7 @@
         <v>76.544295936317098</v>
       </c>
     </row>
-    <row r="95" spans="1:38" hidden="1">
+    <row r="95" spans="1:38">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -5486,7 +5485,7 @@
         <v>78.395165078782483</v>
       </c>
     </row>
-    <row r="96" spans="1:38" hidden="1">
+    <row r="96" spans="1:38">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -5561,7 +5560,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="97" spans="1:38" hidden="1">
+    <row r="97" spans="1:38">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -5596,7 +5595,7 @@
         <v>16.063897410030918</v>
       </c>
       <c r="N97">
-        <v>471.85749999999996</v>
+        <v>459.22249999999997</v>
       </c>
       <c r="O97">
         <v>27.694723136065807</v>
@@ -5652,7 +5651,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="98" spans="1:38" hidden="1">
+    <row r="98" spans="1:38">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -5672,7 +5671,7 @@
         <v>78.90521095393791</v>
       </c>
     </row>
-    <row r="99" spans="1:38" hidden="1">
+    <row r="99" spans="1:38">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -5695,7 +5694,7 @@
         <v>1.2918720988872958</v>
       </c>
     </row>
-    <row r="100" spans="1:38" hidden="1">
+    <row r="100" spans="1:38">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>1.9942853810717764</v>
       </c>
     </row>
-    <row r="101" spans="1:38" hidden="1">
+    <row r="101" spans="1:38">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -5738,7 +5737,7 @@
         <v>8.943632970503522</v>
       </c>
     </row>
-    <row r="102" spans="1:38" hidden="1">
+    <row r="102" spans="1:38">
       <c r="A102" t="s">
         <v>14</v>
       </c>
@@ -5773,7 +5772,7 @@
         <v>12.746311884881264</v>
       </c>
       <c r="N102">
-        <v>238.96750000000003</v>
+        <v>144.10750000000002</v>
       </c>
       <c r="O102">
         <v>18.699014401388443</v>
@@ -5813,7 +5812,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="103" spans="1:38" hidden="1">
+    <row r="103" spans="1:38">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -5836,7 +5835,7 @@
         <v>1.3264114341405446</v>
       </c>
     </row>
-    <row r="104" spans="1:38" hidden="1">
+    <row r="104" spans="1:38">
       <c r="A104" t="s">
         <v>14</v>
       </c>
@@ -5856,7 +5855,7 @@
         <v>52.64872213484513</v>
       </c>
     </row>
-    <row r="105" spans="1:38" hidden="1">
+    <row r="105" spans="1:38">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -5939,7 +5938,7 @@
         <v>6.8999999999999995</v>
       </c>
     </row>
-    <row r="106" spans="1:38" hidden="1">
+    <row r="106" spans="1:38">
       <c r="A106" t="s">
         <v>14</v>
       </c>
@@ -5959,7 +5958,7 @@
         <v>70.941218291500888</v>
       </c>
     </row>
-    <row r="107" spans="1:38" hidden="1">
+    <row r="107" spans="1:38">
       <c r="A107" t="s">
         <v>14</v>
       </c>
@@ -5979,7 +5978,7 @@
         <v>72.649098815351806</v>
       </c>
     </row>
-    <row r="108" spans="1:38" hidden="1">
+    <row r="108" spans="1:38">
       <c r="A108" t="s">
         <v>14</v>
       </c>
@@ -6054,7 +6053,7 @@
         <v>10.875</v>
       </c>
     </row>
-    <row r="109" spans="1:38" hidden="1">
+    <row r="109" spans="1:38">
       <c r="A109" t="s">
         <v>14</v>
       </c>
@@ -6077,7 +6076,7 @@
         <v>0.76863750101380335</v>
       </c>
     </row>
-    <row r="110" spans="1:38" hidden="1">
+    <row r="110" spans="1:38">
       <c r="A110" t="s">
         <v>14</v>
       </c>
@@ -6112,7 +6111,7 @@
         <v>15.437913287315187</v>
       </c>
       <c r="N110">
-        <v>406.185</v>
+        <v>398.56</v>
       </c>
       <c r="O110">
         <v>20.54026837701975</v>
@@ -6174,7 +6173,7 @@
         <v>13.85</v>
       </c>
     </row>
-    <row r="111" spans="1:38" hidden="1">
+    <row r="111" spans="1:38">
       <c r="A111" t="s">
         <v>14</v>
       </c>
@@ -6197,7 +6196,7 @@
         <v>6.4700562743368648</v>
       </c>
     </row>
-    <row r="112" spans="1:38" hidden="1">
+    <row r="112" spans="1:38">
       <c r="A112" t="s">
         <v>14</v>
       </c>
@@ -6232,7 +6231,7 @@
         <v>4.1803907313390392</v>
       </c>
       <c r="N112">
-        <v>163.48999999999998</v>
+        <v>94.9</v>
       </c>
       <c r="O112">
         <v>8.9326162647532428</v>
@@ -6272,7 +6271,7 @@
         <v>4.2750000000000004</v>
       </c>
     </row>
-    <row r="113" spans="1:38" hidden="1">
+    <row r="113" spans="1:38">
       <c r="A113" t="s">
         <v>14</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>3.9789903949757224</v>
       </c>
     </row>
-    <row r="114" spans="1:38" hidden="1">
+    <row r="114" spans="1:38">
       <c r="A114" t="s">
         <v>14</v>
       </c>
@@ -6378,7 +6377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:38" hidden="1">
+    <row r="115" spans="1:38">
       <c r="A115" t="s">
         <v>14</v>
       </c>
@@ -6398,7 +6397,7 @@
         <v>68.774326090449534</v>
       </c>
     </row>
-    <row r="116" spans="1:38" hidden="1">
+    <row r="116" spans="1:38">
       <c r="A116" t="s">
         <v>14</v>
       </c>
@@ -6418,7 +6417,7 @@
         <v>78.929015965050638</v>
       </c>
     </row>
-    <row r="117" spans="1:38" hidden="1">
+    <row r="117" spans="1:38">
       <c r="A117" t="s">
         <v>14</v>
       </c>
@@ -6499,7 +6498,7 @@
         <v>10.433333333333332</v>
       </c>
     </row>
-    <row r="118" spans="1:38" hidden="1">
+    <row r="118" spans="1:38">
       <c r="A118" t="s">
         <v>14</v>
       </c>
@@ -6522,7 +6521,7 @@
         <v>5.3316111861686615</v>
       </c>
     </row>
-    <row r="119" spans="1:38" hidden="1">
+    <row r="119" spans="1:38">
       <c r="A119" t="s">
         <v>14</v>
       </c>
@@ -6551,7 +6550,7 @@
         <v>19.93952711742854</v>
       </c>
       <c r="N119">
-        <v>660.83249999999998</v>
+        <v>630.0575</v>
       </c>
       <c r="O119">
         <v>57.167892850066451</v>
@@ -6617,7 +6616,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row r="120" spans="1:38" hidden="1">
+    <row r="120" spans="1:38">
       <c r="A120" t="s">
         <v>14</v>
       </c>
@@ -6692,7 +6691,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="121" spans="1:38" hidden="1">
+    <row r="121" spans="1:38">
       <c r="A121" t="s">
         <v>14</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>3.6117033768259006</v>
       </c>
     </row>
-    <row r="122" spans="1:38" hidden="1">
+    <row r="122" spans="1:38">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -6738,7 +6737,7 @@
         <v>2.025194891309293</v>
       </c>
     </row>
-    <row r="123" spans="1:38" hidden="1">
+    <row r="123" spans="1:38">
       <c r="A123" t="s">
         <v>14</v>
       </c>
@@ -6811,7 +6810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="124" spans="1:38" hidden="1">
+    <row r="124" spans="1:38">
       <c r="A124" t="s">
         <v>14</v>
       </c>
@@ -6834,7 +6833,7 @@
         <v>5.485209168157211</v>
       </c>
     </row>
-    <row r="125" spans="1:38" hidden="1">
+    <row r="125" spans="1:38">
       <c r="A125" t="s">
         <v>14</v>
       </c>
@@ -6909,7 +6908,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="126" spans="1:38" hidden="1">
+    <row r="126" spans="1:38">
       <c r="A126" t="s">
         <v>14</v>
       </c>
@@ -6932,7 +6931,7 @@
         <v>2.9032155393600219</v>
       </c>
     </row>
-    <row r="127" spans="1:38" hidden="1">
+    <row r="127" spans="1:38">
       <c r="A127" t="s">
         <v>14</v>
       </c>
@@ -6967,7 +6966,7 @@
         <v>5.1936523757370905</v>
       </c>
       <c r="N127">
-        <v>360.4325</v>
+        <v>355.54500000000007</v>
       </c>
       <c r="O127">
         <v>117.66625729685637</v>
@@ -7023,7 +7022,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="128" spans="1:38" hidden="1">
+    <row r="128" spans="1:38">
       <c r="A128" t="s">
         <v>14</v>
       </c>
@@ -7046,7 +7045,7 @@
         <v>5.8459521714162985</v>
       </c>
     </row>
-    <row r="129" spans="1:38" hidden="1">
+    <row r="129" spans="1:38">
       <c r="A129" t="s">
         <v>14</v>
       </c>
@@ -7069,7 +7068,7 @@
         <v>4.498142685492609</v>
       </c>
     </row>
-    <row r="130" spans="1:38" hidden="1">
+    <row r="130" spans="1:38">
       <c r="A130" t="s">
         <v>14</v>
       </c>
@@ -7134,7 +7133,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="131" spans="1:38" hidden="1">
+    <row r="131" spans="1:38">
       <c r="A131" t="s">
         <v>14</v>
       </c>
@@ -7157,7 +7156,7 @@
         <v>3.2760497556779269</v>
       </c>
     </row>
-    <row r="132" spans="1:38" hidden="1">
+    <row r="132" spans="1:38">
       <c r="A132" t="s">
         <v>14</v>
       </c>
@@ -7240,7 +7239,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="133" spans="1:38" hidden="1">
+    <row r="133" spans="1:38">
       <c r="A133" t="s">
         <v>14</v>
       </c>
@@ -7263,7 +7262,7 @@
         <v>2.0361737340178747</v>
       </c>
     </row>
-    <row r="134" spans="1:38" hidden="1">
+    <row r="134" spans="1:38">
       <c r="A134" t="s">
         <v>14</v>
       </c>
@@ -7344,7 +7343,7 @@
         <v>11.475</v>
       </c>
     </row>
-    <row r="135" spans="1:38" hidden="1">
+    <row r="135" spans="1:38">
       <c r="A135" t="s">
         <v>14</v>
       </c>
@@ -7367,7 +7366,7 @@
         <v>2.3566347287549427</v>
       </c>
     </row>
-    <row r="136" spans="1:38" hidden="1">
+    <row r="136" spans="1:38">
       <c r="A136" t="s">
         <v>14</v>
       </c>
@@ -7390,7 +7389,7 @@
         <v>2.8488164720094478</v>
       </c>
     </row>
-    <row r="137" spans="1:38" hidden="1">
+    <row r="137" spans="1:38">
       <c r="A137" t="s">
         <v>14</v>
       </c>
@@ -7419,7 +7418,7 @@
         <v>25.013407238252576</v>
       </c>
       <c r="N137">
-        <v>406.20499999999993</v>
+        <v>400.0625</v>
       </c>
       <c r="O137">
         <v>77.037978675023339</v>
@@ -7485,7 +7484,7 @@
         <v>12.525</v>
       </c>
     </row>
-    <row r="138" spans="1:38" hidden="1">
+    <row r="138" spans="1:38">
       <c r="A138" t="s">
         <v>14</v>
       </c>
@@ -7508,7 +7507,7 @@
         <v>4.5511836838559532</v>
       </c>
     </row>
-    <row r="139" spans="1:38" hidden="1">
+    <row r="139" spans="1:38">
       <c r="A139" t="s">
         <v>14</v>
       </c>
@@ -7583,7 +7582,7 @@
         <v>4.4499999999999993</v>
       </c>
     </row>
-    <row r="140" spans="1:38" hidden="1">
+    <row r="140" spans="1:38">
       <c r="A140" t="s">
         <v>14</v>
       </c>
@@ -7606,7 +7605,7 @@
         <v>2.9150963623880548</v>
       </c>
     </row>
-    <row r="141" spans="1:38" hidden="1">
+    <row r="141" spans="1:38">
       <c r="A141" t="s">
         <v>14</v>
       </c>
@@ -7689,7 +7688,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="142" spans="1:38" hidden="1">
+    <row r="142" spans="1:38">
       <c r="A142" t="s">
         <v>14</v>
       </c>
@@ -7712,7 +7711,7 @@
         <v>2.6783143273519876</v>
       </c>
     </row>
-    <row r="143" spans="1:38" hidden="1">
+    <row r="143" spans="1:38">
       <c r="A143" t="s">
         <v>14</v>
       </c>
@@ -7793,7 +7792,7 @@
         <v>10.899999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:38" hidden="1">
+    <row r="144" spans="1:38">
       <c r="A144" t="s">
         <v>14</v>
       </c>
@@ -7816,7 +7815,7 @@
         <v>3.5724818750005722</v>
       </c>
     </row>
-    <row r="145" spans="1:38" hidden="1">
+    <row r="145" spans="1:38">
       <c r="A145" t="s">
         <v>14</v>
       </c>
@@ -7839,7 +7838,7 @@
         <v>0.87832205022106069</v>
       </c>
     </row>
-    <row r="146" spans="1:38" hidden="1">
+    <row r="146" spans="1:38">
       <c r="A146" t="s">
         <v>14</v>
       </c>
@@ -7868,7 +7867,7 @@
         <v>25.62977707504826</v>
       </c>
       <c r="N146">
-        <v>506.52250000000004</v>
+        <v>492.4975</v>
       </c>
       <c r="O146">
         <v>52.237185569764321</v>
@@ -7934,7 +7933,7 @@
         <v>13.65</v>
       </c>
     </row>
-    <row r="147" spans="1:38" hidden="1">
+    <row r="147" spans="1:38">
       <c r="A147" t="s">
         <v>14</v>
       </c>
@@ -7999,7 +7998,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="148" spans="1:38" hidden="1">
+    <row r="148" spans="1:38">
       <c r="A148" t="s">
         <v>14</v>
       </c>
@@ -8022,7 +8021,7 @@
         <v>1.6346540621764984</v>
       </c>
     </row>
-    <row r="149" spans="1:38" hidden="1">
+    <row r="149" spans="1:38">
       <c r="A149" t="s">
         <v>14</v>
       </c>
@@ -8045,7 +8044,7 @@
         <v>1.4736836772398236</v>
       </c>
     </row>
-    <row r="150" spans="1:38" hidden="1">
+    <row r="150" spans="1:38">
       <c r="A150" t="s">
         <v>14</v>
       </c>
@@ -8068,7 +8067,7 @@
         <v>2.5732585159995178</v>
       </c>
     </row>
-    <row r="151" spans="1:38" hidden="1">
+    <row r="151" spans="1:38">
       <c r="A151" t="s">
         <v>14</v>
       </c>
@@ -8091,7 +8090,7 @@
         <v>4.4618262568565408</v>
       </c>
     </row>
-    <row r="152" spans="1:38" hidden="1">
+    <row r="152" spans="1:38">
       <c r="A152" t="s">
         <v>14</v>
       </c>
@@ -8174,7 +8173,7 @@
         <v>7.1749999999999989</v>
       </c>
     </row>
-    <row r="153" spans="1:38" hidden="1">
+    <row r="153" spans="1:38">
       <c r="A153" t="s">
         <v>14</v>
       </c>
@@ -8194,7 +8193,7 @@
         <v>13.804713804713813</v>
       </c>
     </row>
-    <row r="154" spans="1:38" hidden="1">
+    <row r="154" spans="1:38">
       <c r="A154" t="s">
         <v>14</v>
       </c>
@@ -8269,7 +8268,7 @@
         <v>12.400000000000002</v>
       </c>
     </row>
-    <row r="155" spans="1:38" hidden="1">
+    <row r="155" spans="1:38">
       <c r="A155" t="s">
         <v>14</v>
       </c>
@@ -8292,7 +8291,7 @@
         <v>3.2299049259008243</v>
       </c>
     </row>
-    <row r="156" spans="1:38" hidden="1">
+    <row r="156" spans="1:38">
       <c r="A156" t="s">
         <v>14</v>
       </c>
@@ -8315,7 +8314,7 @@
         <v>4.6284358100428769</v>
       </c>
     </row>
-    <row r="157" spans="1:38" hidden="1">
+    <row r="157" spans="1:38">
       <c r="A157" t="s">
         <v>14</v>
       </c>
@@ -8400,7 +8399,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="1:38" hidden="1">
+    <row r="158" spans="1:38">
       <c r="A158" t="s">
         <v>14</v>
       </c>
@@ -8423,7 +8422,7 @@
         <v>2.0010476690249828</v>
       </c>
     </row>
-    <row r="159" spans="1:38" hidden="1">
+    <row r="159" spans="1:38">
       <c r="A159" t="s">
         <v>14</v>
       </c>
@@ -8446,7 +8445,7 @@
         <v>0.84128488525335965</v>
       </c>
     </row>
-    <row r="160" spans="1:38" hidden="1">
+    <row r="160" spans="1:38">
       <c r="A160" t="s">
         <v>14</v>
       </c>
@@ -8511,7 +8510,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="161" spans="1:38" hidden="1">
+    <row r="161" spans="1:38">
       <c r="A161" t="s">
         <v>14</v>
       </c>
@@ -8534,7 +8533,7 @@
         <v>2.1356954359294411</v>
       </c>
     </row>
-    <row r="162" spans="1:38" hidden="1">
+    <row r="162" spans="1:38">
       <c r="A162" t="s">
         <v>14</v>
       </c>
@@ -8557,7 +8556,7 @@
         <v>3.9112334520629624</v>
       </c>
     </row>
-    <row r="163" spans="1:38" hidden="1">
+    <row r="163" spans="1:38">
       <c r="A163" t="s">
         <v>14</v>
       </c>
@@ -8578,7 +8577,7 @@
       </c>
       <c r="AC163" s="14"/>
     </row>
-    <row r="164" spans="1:38" hidden="1">
+    <row r="164" spans="1:38">
       <c r="A164" t="s">
         <v>14</v>
       </c>
@@ -8601,7 +8600,7 @@
         <v>2.6847889217066414</v>
       </c>
     </row>
-    <row r="165" spans="1:38" hidden="1">
+    <row r="165" spans="1:38">
       <c r="A165" t="s">
         <v>14</v>
       </c>
@@ -8621,7 +8620,7 @@
         <v>50.741447658199966</v>
       </c>
     </row>
-    <row r="166" spans="1:38" hidden="1">
+    <row r="166" spans="1:38">
       <c r="A166" t="s">
         <v>14</v>
       </c>
@@ -8644,7 +8643,7 @@
         <v>5.4663787711219589</v>
       </c>
     </row>
-    <row r="167" spans="1:38" hidden="1">
+    <row r="167" spans="1:38">
       <c r="A167" t="s">
         <v>14</v>
       </c>
@@ -8727,7 +8726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:38" hidden="1">
+    <row r="168" spans="1:38">
       <c r="A168" t="s">
         <v>14</v>
       </c>
@@ -8792,7 +8791,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="169" spans="1:38" hidden="1">
+    <row r="169" spans="1:38">
       <c r="A169" t="s">
         <v>14</v>
       </c>
@@ -8815,7 +8814,7 @@
         <v>4.7422054179886226</v>
       </c>
     </row>
-    <row r="170" spans="1:38" hidden="1">
+    <row r="170" spans="1:38">
       <c r="A170" t="s">
         <v>14</v>
       </c>
@@ -8838,7 +8837,7 @@
         <v>3.4965156692075374</v>
       </c>
     </row>
-    <row r="171" spans="1:38" hidden="1">
+    <row r="171" spans="1:38">
       <c r="A171" t="s">
         <v>14</v>
       </c>
@@ -8861,7 +8860,7 @@
         <v>2.000056003418893</v>
       </c>
     </row>
-    <row r="172" spans="1:38" hidden="1">
+    <row r="172" spans="1:38">
       <c r="A172" t="s">
         <v>14</v>
       </c>
@@ -8890,7 +8889,7 @@
         <v>11.175157344156974</v>
       </c>
       <c r="N172">
-        <v>782.49499999999989</v>
+        <v>751.48249999999996</v>
       </c>
       <c r="O172">
         <v>203.9830383675729</v>
@@ -8956,7 +8955,7 @@
         <v>7.3500000000000014</v>
       </c>
     </row>
-    <row r="173" spans="1:38" hidden="1">
+    <row r="173" spans="1:38">
       <c r="A173" t="s">
         <v>14</v>
       </c>
@@ -8979,7 +8978,7 @@
         <v>0.74353522578927023</v>
       </c>
     </row>
-    <row r="174" spans="1:38" hidden="1">
+    <row r="174" spans="1:38">
       <c r="A174" t="s">
         <v>14</v>
       </c>
@@ -9044,7 +9043,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="175" spans="1:38" hidden="1">
+    <row r="175" spans="1:38">
       <c r="A175" t="s">
         <v>14</v>
       </c>
@@ -9067,7 +9066,7 @@
         <v>0.74509690370666115</v>
       </c>
     </row>
-    <row r="176" spans="1:38" hidden="1">
+    <row r="176" spans="1:38">
       <c r="A176" t="s">
         <v>14</v>
       </c>
@@ -9090,7 +9089,7 @@
         <v>2.2365871765787624</v>
       </c>
     </row>
-    <row r="177" spans="1:38" hidden="1">
+    <row r="177" spans="1:38">
       <c r="A177" t="s">
         <v>14</v>
       </c>
@@ -9113,7 +9112,7 @@
         <v>2.6256045624529158</v>
       </c>
     </row>
-    <row r="178" spans="1:38" hidden="1">
+    <row r="178" spans="1:38">
       <c r="A178" t="s">
         <v>14</v>
       </c>
@@ -9190,7 +9189,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="179" spans="1:38" hidden="1">
+    <row r="179" spans="1:38">
       <c r="A179" t="s">
         <v>14</v>
       </c>
@@ -9213,7 +9212,7 @@
         <v>1.8841088733970519</v>
       </c>
     </row>
-    <row r="180" spans="1:38" hidden="1">
+    <row r="180" spans="1:38">
       <c r="A180" t="s">
         <v>14</v>
       </c>
@@ -9288,7 +9287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:38" hidden="1">
+    <row r="181" spans="1:38">
       <c r="A181" t="s">
         <v>14</v>
       </c>
@@ -9311,7 +9310,7 @@
         <v>7.1589111598088291</v>
       </c>
     </row>
-    <row r="182" spans="1:38" hidden="1">
+    <row r="182" spans="1:38">
       <c r="A182" t="s">
         <v>14</v>
       </c>
@@ -9334,7 +9333,7 @@
         <v>1.4286241964891497</v>
       </c>
     </row>
-    <row r="183" spans="1:38" hidden="1">
+    <row r="183" spans="1:38">
       <c r="A183" t="s">
         <v>14</v>
       </c>
@@ -9357,7 +9356,7 @@
         <v>5.1947128630896646</v>
       </c>
     </row>
-    <row r="184" spans="1:38" hidden="1">
+    <row r="184" spans="1:38">
       <c r="A184" t="s">
         <v>14</v>
       </c>
@@ -9386,7 +9385,7 @@
         <v>27.729138817917406</v>
       </c>
       <c r="N184">
-        <v>507.55</v>
+        <v>485.6</v>
       </c>
       <c r="O184">
         <v>110.958464526146</v>
@@ -9452,7 +9451,7 @@
         <v>11.05</v>
       </c>
     </row>
-    <row r="185" spans="1:38" hidden="1">
+    <row r="185" spans="1:38">
       <c r="A185" t="s">
         <v>14</v>
       </c>
@@ -9517,7 +9516,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="186" spans="1:38" hidden="1">
+    <row r="186" spans="1:38">
       <c r="A186" t="s">
         <v>14</v>
       </c>
@@ -9540,7 +9539,7 @@
         <v>0.9394940748123165</v>
       </c>
     </row>
-    <row r="187" spans="1:38" hidden="1">
+    <row r="187" spans="1:38">
       <c r="A187" t="s">
         <v>14</v>
       </c>
@@ -9560,7 +9559,7 @@
         <v>1.936894720399863</v>
       </c>
     </row>
-    <row r="188" spans="1:38" hidden="1">
+    <row r="188" spans="1:38">
       <c r="A188" t="s">
         <v>14</v>
       </c>
@@ -9583,7 +9582,7 @@
         <v>1.4075989132976168</v>
       </c>
     </row>
-    <row r="189" spans="1:38" hidden="1">
+    <row r="189" spans="1:38">
       <c r="A189" t="s">
         <v>14</v>
       </c>
@@ -9606,7 +9605,7 @@
         <v>4.1724876352853677</v>
       </c>
     </row>
-    <row r="190" spans="1:38" hidden="1">
+    <row r="190" spans="1:38">
       <c r="A190" t="s">
         <v>14</v>
       </c>
@@ -9689,7 +9688,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="191" spans="1:38" hidden="1">
+    <row r="191" spans="1:38">
       <c r="A191" t="s">
         <v>14</v>
       </c>
@@ -9764,7 +9763,7 @@
         <v>5.3250000000000002</v>
       </c>
     </row>
-    <row r="192" spans="1:38" hidden="1">
+    <row r="192" spans="1:38">
       <c r="A192" t="s">
         <v>14</v>
       </c>
@@ -9787,7 +9786,7 @@
         <v>2.2991176144107279</v>
       </c>
     </row>
-    <row r="193" spans="1:38" hidden="1">
+    <row r="193" spans="1:38">
       <c r="A193" t="s">
         <v>14</v>
       </c>
@@ -9810,7 +9809,7 @@
         <v>2.6491308633039106</v>
       </c>
     </row>
-    <row r="194" spans="1:38" hidden="1">
+    <row r="194" spans="1:38">
       <c r="A194" t="s">
         <v>14</v>
       </c>
@@ -9891,7 +9890,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="195" spans="1:38" hidden="1">
+    <row r="195" spans="1:38">
       <c r="A195" t="s">
         <v>14</v>
       </c>
@@ -9914,7 +9913,7 @@
         <v>3.8274828439374287</v>
       </c>
     </row>
-    <row r="196" spans="1:38" hidden="1">
+    <row r="196" spans="1:38">
       <c r="A196" t="s">
         <v>14</v>
       </c>
@@ -9937,7 +9936,7 @@
         <v>2.510627081489849</v>
       </c>
     </row>
-    <row r="197" spans="1:38" hidden="1">
+    <row r="197" spans="1:38">
       <c r="A197" t="s">
         <v>14</v>
       </c>
@@ -10002,7 +10001,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="198" spans="1:38" hidden="1">
+    <row r="198" spans="1:38">
       <c r="A198" t="s">
         <v>14</v>
       </c>
@@ -10022,7 +10021,7 @@
         <v>1.5370941600878325</v>
       </c>
     </row>
-    <row r="199" spans="1:38" hidden="1">
+    <row r="199" spans="1:38">
       <c r="A199" t="s">
         <v>14</v>
       </c>
@@ -10045,7 +10044,7 @@
         <v>0.59463305412538903</v>
       </c>
     </row>
-    <row r="200" spans="1:38" hidden="1">
+    <row r="200" spans="1:38">
       <c r="A200" t="s">
         <v>14</v>
       </c>
@@ -10068,7 +10067,7 @@
         <v>3.7111956028324835</v>
       </c>
     </row>
-    <row r="201" spans="1:38" hidden="1">
+    <row r="201" spans="1:38">
       <c r="A201" t="s">
         <v>14</v>
       </c>
@@ -10088,7 +10087,7 @@
         <v>8.1466512702078546</v>
       </c>
     </row>
-    <row r="202" spans="1:38" hidden="1">
+    <row r="202" spans="1:38">
       <c r="A202" t="s">
         <v>14</v>
       </c>
@@ -10171,7 +10170,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="203" spans="1:38" hidden="1">
+    <row r="203" spans="1:38">
       <c r="A203" t="s">
         <v>14</v>
       </c>
@@ -10236,7 +10235,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:38" hidden="1">
+    <row r="204" spans="1:38">
       <c r="A204" t="s">
         <v>14</v>
       </c>
@@ -10259,7 +10258,7 @@
         <v>3.6048651545304731</v>
       </c>
     </row>
-    <row r="205" spans="1:38" hidden="1">
+    <row r="205" spans="1:38">
       <c r="A205" t="s">
         <v>14</v>
       </c>
@@ -10282,7 +10281,7 @@
         <v>2.3095845924176341</v>
       </c>
     </row>
-    <row r="206" spans="1:38" hidden="1">
+    <row r="206" spans="1:38">
       <c r="A206" t="s">
         <v>14</v>
       </c>
@@ -10305,7 +10304,7 @@
         <v>4.6688599058321465</v>
       </c>
     </row>
-    <row r="207" spans="1:38" hidden="1">
+    <row r="207" spans="1:38">
       <c r="A207" t="s">
         <v>14</v>
       </c>
@@ -10334,7 +10333,7 @@
         <v>7.9324285636031213</v>
       </c>
       <c r="N207">
-        <v>239.03000000000003</v>
+        <v>215.01249999999999</v>
       </c>
       <c r="O207">
         <v>10.67973548361539</v>
@@ -10400,7 +10399,7 @@
         <v>5.0250000000000004</v>
       </c>
     </row>
-    <row r="208" spans="1:38" hidden="1">
+    <row r="208" spans="1:38">
       <c r="A208" t="s">
         <v>14</v>
       </c>
@@ -10423,7 +10422,7 @@
         <v>1.6851677522614044</v>
       </c>
     </row>
-    <row r="209" spans="1:38" hidden="1">
+    <row r="209" spans="1:38">
       <c r="A209" t="s">
         <v>14</v>
       </c>
@@ -10459,7 +10458,7 @@
         <v>3.2088107869842566</v>
       </c>
       <c r="N209">
-        <v>31.502499999999998</v>
+        <v>30.85</v>
       </c>
       <c r="O209">
         <v>2.5524269496566032</v>
@@ -10489,7 +10488,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="210" spans="1:38" hidden="1">
+    <row r="210" spans="1:38">
       <c r="A210" t="s">
         <v>14</v>
       </c>
@@ -10512,7 +10511,7 @@
         <v>2.1218261966437177</v>
       </c>
     </row>
-    <row r="211" spans="1:38" hidden="1">
+    <row r="211" spans="1:38">
       <c r="A211" t="s">
         <v>14</v>
       </c>
@@ -10535,7 +10534,7 @@
         <v>0.9808917672312738</v>
       </c>
     </row>
-    <row r="212" spans="1:38" hidden="1">
+    <row r="212" spans="1:38">
       <c r="A212" t="s">
         <v>14</v>
       </c>
@@ -10558,7 +10557,7 @@
         <v>4.0670957683044096</v>
       </c>
     </row>
-    <row r="213" spans="1:38" hidden="1">
+    <row r="213" spans="1:38">
       <c r="A213" t="s">
         <v>14</v>
       </c>
@@ -10595,7 +10594,7 @@
         <v>1.1832934265571331</v>
       </c>
       <c r="N213">
-        <v>77.259999999999991</v>
+        <v>67.27</v>
       </c>
       <c r="O213">
         <v>3.0600282542268089</v>
@@ -10635,7 +10634,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="214" spans="1:38" hidden="1">
+    <row r="214" spans="1:38">
       <c r="A214" t="s">
         <v>14</v>
       </c>
@@ -10664,7 +10663,7 @@
         <v>6.1684011637268403</v>
       </c>
       <c r="N214">
-        <v>210.45500000000001</v>
+        <v>87.94</v>
       </c>
       <c r="O214">
         <v>14.298896519195681</v>
@@ -10711,7 +10710,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="215" spans="1:38" hidden="1">
+    <row r="215" spans="1:38">
       <c r="A215" t="s">
         <v>14</v>
       </c>
@@ -10734,7 +10733,7 @@
         <v>3.6540452544246205</v>
       </c>
     </row>
-    <row r="216" spans="1:38" hidden="1">
+    <row r="216" spans="1:38">
       <c r="A216" t="s">
         <v>14</v>
       </c>
@@ -10757,7 +10756,7 @@
         <v>2.6923475326620641</v>
       </c>
     </row>
-    <row r="217" spans="1:38" hidden="1">
+    <row r="217" spans="1:38">
       <c r="A217" t="s">
         <v>14</v>
       </c>
@@ -10780,7 +10779,7 @@
         <v>5.429230338369984</v>
       </c>
     </row>
-    <row r="218" spans="1:38" hidden="1">
+    <row r="218" spans="1:38">
       <c r="A218" t="s">
         <v>14</v>
       </c>
@@ -10809,7 +10808,7 @@
         <v>5.4850377923340945</v>
       </c>
       <c r="N218">
-        <v>507.55</v>
+        <v>150.84</v>
       </c>
       <c r="O218">
         <v>23.831171114040238</v>
@@ -10876,7 +10875,7 @@
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="219" spans="1:38" hidden="1">
+    <row r="219" spans="1:38">
       <c r="A219" t="s">
         <v>14</v>
       </c>
@@ -10941,7 +10940,7 @@
         <v>4.5500000000000007</v>
       </c>
     </row>
-    <row r="220" spans="1:38" hidden="1">
+    <row r="220" spans="1:38">
       <c r="A220" t="s">
         <v>14</v>
       </c>
@@ -11024,7 +11023,7 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="221" spans="1:38" hidden="1">
+    <row r="221" spans="1:38">
       <c r="A221" t="s">
         <v>14</v>
       </c>
@@ -11148,7 +11147,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="223" spans="1:38" hidden="1">
+    <row r="223" spans="1:38">
       <c r="A223" t="s">
         <v>14</v>
       </c>
@@ -11212,7 +11211,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="224" spans="1:38" hidden="1">
+    <row r="224" spans="1:38">
       <c r="A224" t="s">
         <v>14</v>
       </c>
@@ -11294,7 +11293,7 @@
         <v>12.049999999999999</v>
       </c>
     </row>
-    <row r="225" spans="1:38" hidden="1">
+    <row r="225" spans="1:38">
       <c r="A225" t="s">
         <v>14</v>
       </c>
@@ -11417,7 +11416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="227" spans="1:38" hidden="1">
+    <row r="227" spans="1:38">
       <c r="A227" t="s">
         <v>14</v>
       </c>
@@ -11481,7 +11480,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="228" spans="1:38" hidden="1">
+    <row r="228" spans="1:38">
       <c r="A228" t="s">
         <v>14</v>
       </c>
@@ -11563,7 +11562,7 @@
         <v>5.9249999999999998</v>
       </c>
     </row>
-    <row r="229" spans="1:38" hidden="1">
+    <row r="229" spans="1:38">
       <c r="A229" t="s">
         <v>14</v>
       </c>
@@ -11686,7 +11685,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="231" spans="1:38" hidden="1">
+    <row r="231" spans="1:38">
       <c r="A231" t="s">
         <v>14</v>
       </c>
@@ -11750,7 +11749,7 @@
         <v>4.335</v>
       </c>
     </row>
-    <row r="232" spans="1:38" hidden="1">
+    <row r="232" spans="1:38">
       <c r="A232" t="s">
         <v>14</v>
       </c>
@@ -11832,7 +11831,7 @@
         <v>6.9249999999999989</v>
       </c>
     </row>
-    <row r="233" spans="1:38" hidden="1">
+    <row r="233" spans="1:38">
       <c r="A233" t="s">
         <v>14</v>
       </c>
@@ -11955,7 +11954,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="235" spans="1:38" hidden="1">
+    <row r="235" spans="1:38">
       <c r="A235" t="s">
         <v>14</v>
       </c>
@@ -12018,7 +12017,7 @@
         <v>4.8666666666666671</v>
       </c>
     </row>
-    <row r="236" spans="1:38" hidden="1">
+    <row r="236" spans="1:38">
       <c r="A236" t="s">
         <v>14</v>
       </c>
@@ -12099,7 +12098,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="237" spans="1:38" hidden="1">
+    <row r="237" spans="1:38">
       <c r="A237" t="s">
         <v>14</v>
       </c>
@@ -12222,7 +12221,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="239" spans="1:38" hidden="1">
+    <row r="239" spans="1:38">
       <c r="A239" t="s">
         <v>14</v>
       </c>
@@ -12285,7 +12284,7 @@
         <v>3.8499999999999996</v>
       </c>
     </row>
-    <row r="240" spans="1:38" hidden="1">
+    <row r="240" spans="1:38">
       <c r="A240" t="s">
         <v>14</v>
       </c>
@@ -12366,7 +12365,7 @@
         <v>6.0749999999999993</v>
       </c>
     </row>
-    <row r="241" spans="1:38" hidden="1">
+    <row r="241" spans="1:38">
       <c r="A241" t="s">
         <v>14</v>
       </c>
@@ -12489,7 +12488,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="243" spans="1:38" hidden="1">
+    <row r="243" spans="1:38">
       <c r="A243" t="s">
         <v>14</v>
       </c>
@@ -12570,7 +12569,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="244" spans="1:38" hidden="1">
+    <row r="244" spans="1:38">
       <c r="A244" t="s">
         <v>14</v>
       </c>
@@ -12659,7 +12658,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="245" spans="1:38" hidden="1">
+    <row r="245" spans="1:38">
       <c r="A245" t="s">
         <v>14</v>
       </c>
@@ -12828,7 +12827,7 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="247" spans="1:38" hidden="1">
+    <row r="247" spans="1:38">
       <c r="A247" t="s">
         <v>14</v>
       </c>
@@ -12909,7 +12908,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="248" spans="1:38" hidden="1">
+    <row r="248" spans="1:38">
       <c r="A248" t="s">
         <v>14</v>
       </c>
@@ -12998,7 +12997,7 @@
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="249" spans="1:38" hidden="1">
+    <row r="249" spans="1:38">
       <c r="A249" t="s">
         <v>14</v>
       </c>
@@ -13167,7 +13166,7 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="251" spans="1:38" hidden="1">
+    <row r="251" spans="1:38">
       <c r="A251" t="s">
         <v>14</v>
       </c>
@@ -13248,7 +13247,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="252" spans="1:38" hidden="1">
+    <row r="252" spans="1:38">
       <c r="A252" t="s">
         <v>14</v>
       </c>
@@ -13337,7 +13336,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="253" spans="1:38" hidden="1">
+    <row r="253" spans="1:38">
       <c r="A253" t="s">
         <v>14</v>
       </c>
@@ -13506,7 +13505,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="255" spans="1:38" hidden="1">
+    <row r="255" spans="1:38">
       <c r="A255" t="s">
         <v>14</v>
       </c>
@@ -13587,7 +13586,7 @@
         <v>5.3666666666666671</v>
       </c>
     </row>
-    <row r="256" spans="1:38" hidden="1">
+    <row r="256" spans="1:38">
       <c r="A256" t="s">
         <v>14</v>
       </c>
@@ -13676,7 +13675,7 @@
         <v>5.5500000000000007</v>
       </c>
     </row>
-    <row r="257" spans="1:38" hidden="1">
+    <row r="257" spans="1:38">
       <c r="A257" t="s">
         <v>14</v>
       </c>
@@ -13845,7 +13844,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="259" spans="1:38" hidden="1">
+    <row r="259" spans="1:38">
       <c r="A259" t="s">
         <v>14</v>
       </c>
@@ -13926,7 +13925,7 @@
         <v>7.3000000000000007</v>
       </c>
     </row>
-    <row r="260" spans="1:38" hidden="1">
+    <row r="260" spans="1:38">
       <c r="A260" t="s">
         <v>14</v>
       </c>
@@ -14015,7 +14014,7 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="261" spans="1:38" hidden="1">
+    <row r="261" spans="1:38">
       <c r="A261" t="s">
         <v>14</v>
       </c>
@@ -14184,7 +14183,7 @@
         <v>14.59</v>
       </c>
     </row>
-    <row r="263" spans="1:38" hidden="1">
+    <row r="263" spans="1:38">
       <c r="A263" t="s">
         <v>14</v>
       </c>
@@ -14265,7 +14264,7 @@
         <v>5.4499999999999993</v>
       </c>
     </row>
-    <row r="264" spans="1:38" hidden="1">
+    <row r="264" spans="1:38">
       <c r="A264" t="s">
         <v>14</v>
       </c>
@@ -14354,7 +14353,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="265" spans="1:38" hidden="1">
+    <row r="265" spans="1:38">
       <c r="A265" t="s">
         <v>14</v>
       </c>
@@ -14523,7 +14522,7 @@
         <v>11.324999999999999</v>
       </c>
     </row>
-    <row r="267" spans="1:38" hidden="1">
+    <row r="267" spans="1:38">
       <c r="A267" t="s">
         <v>14</v>
       </c>
@@ -14604,7 +14603,7 @@
         <v>3.1500000000000004</v>
       </c>
     </row>
-    <row r="268" spans="1:38" hidden="1">
+    <row r="268" spans="1:38">
       <c r="A268" t="s">
         <v>14</v>
       </c>
@@ -14693,7 +14692,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="269" spans="1:38" hidden="1">
+    <row r="269" spans="1:38">
       <c r="A269" t="s">
         <v>14</v>
       </c>
@@ -14862,7 +14861,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="271" spans="1:38" hidden="1">
+    <row r="271" spans="1:38">
       <c r="A271" t="s">
         <v>14</v>
       </c>
@@ -14943,7 +14942,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="272" spans="1:38" hidden="1">
+    <row r="272" spans="1:38">
       <c r="A272" t="s">
         <v>14</v>
       </c>
@@ -15032,7 +15031,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="273" spans="1:38" hidden="1">
+    <row r="273" spans="1:38">
       <c r="A273" t="s">
         <v>14</v>
       </c>
@@ -15201,7 +15200,7 @@
         <v>13.8125</v>
       </c>
     </row>
-    <row r="275" spans="1:38" hidden="1">
+    <row r="275" spans="1:38">
       <c r="A275" t="s">
         <v>14</v>
       </c>
@@ -15282,7 +15281,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="276" spans="1:38" hidden="1">
+    <row r="276" spans="1:38">
       <c r="A276" t="s">
         <v>14</v>
       </c>
@@ -15371,7 +15370,7 @@
         <v>7.2000000000000011</v>
       </c>
     </row>
-    <row r="277" spans="1:38" hidden="1">
+    <row r="277" spans="1:38">
       <c r="A277" t="s">
         <v>14</v>
       </c>
@@ -15540,7 +15539,7 @@
         <v>11.15</v>
       </c>
     </row>
-    <row r="279" spans="1:38" hidden="1">
+    <row r="279" spans="1:38">
       <c r="A279" t="s">
         <v>14</v>
       </c>
@@ -15621,7 +15620,7 @@
         <v>2.7249999999999996</v>
       </c>
     </row>
-    <row r="280" spans="1:38" hidden="1">
+    <row r="280" spans="1:38">
       <c r="A280" t="s">
         <v>14</v>
       </c>
@@ -15710,7 +15709,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="281" spans="1:38" hidden="1">
+    <row r="281" spans="1:38">
       <c r="A281" t="s">
         <v>14</v>
       </c>
@@ -15879,7 +15878,7 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="283" spans="1:38" hidden="1">
+    <row r="283" spans="1:38">
       <c r="A283" t="s">
         <v>14</v>
       </c>
@@ -15960,7 +15959,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="284" spans="1:38" hidden="1">
+    <row r="284" spans="1:38">
       <c r="A284" t="s">
         <v>14</v>
       </c>
@@ -16049,7 +16048,7 @@
         <v>7.375</v>
       </c>
     </row>
-    <row r="285" spans="1:38" hidden="1">
+    <row r="285" spans="1:38">
       <c r="A285" t="s">
         <v>14</v>
       </c>
@@ -16218,7 +16217,7 @@
         <v>13.825000000000001</v>
       </c>
     </row>
-    <row r="287" spans="1:38" hidden="1">
+    <row r="287" spans="1:38">
       <c r="A287" t="s">
         <v>14</v>
       </c>
@@ -16299,7 +16298,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="288" spans="1:38" hidden="1">
+    <row r="288" spans="1:38">
       <c r="A288" t="s">
         <v>14</v>
       </c>
@@ -16388,7 +16387,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="289" spans="1:38" hidden="1">
+    <row r="289" spans="1:38">
       <c r="A289" t="s">
         <v>14</v>
       </c>
@@ -16557,7 +16556,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="291" spans="1:38" hidden="1">
+    <row r="291" spans="1:38">
       <c r="A291" t="s">
         <v>14</v>
       </c>
@@ -16604,7 +16603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:38" hidden="1">
+    <row r="292" spans="1:38">
       <c r="A292" t="s">
         <v>14</v>
       </c>
@@ -16651,7 +16650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:38" hidden="1">
+    <row r="293" spans="1:38">
       <c r="A293" t="s">
         <v>14</v>
       </c>
@@ -16698,7 +16697,7 @@
         <v>1.1159030349153662</v>
       </c>
     </row>
-    <row r="294" spans="1:38" hidden="1">
+    <row r="294" spans="1:38">
       <c r="A294" t="s">
         <v>14</v>
       </c>
@@ -16752,7 +16751,7 @@
         <v>19.981315178185927</v>
       </c>
     </row>
-    <row r="295" spans="1:38" hidden="1">
+    <row r="295" spans="1:38">
       <c r="A295" t="s">
         <v>14</v>
       </c>
@@ -16799,7 +16798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:38" hidden="1">
+    <row r="296" spans="1:38">
       <c r="A296" t="s">
         <v>14</v>
       </c>
@@ -16846,7 +16845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:38" hidden="1">
+    <row r="297" spans="1:38">
       <c r="A297" t="s">
         <v>14</v>
       </c>
@@ -16947,7 +16946,7 @@
         <v>25.523318908438497</v>
       </c>
     </row>
-    <row r="299" spans="1:38" hidden="1">
+    <row r="299" spans="1:38">
       <c r="A299" t="s">
         <v>14</v>
       </c>
@@ -16994,7 +16993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:38" hidden="1">
+    <row r="300" spans="1:38">
       <c r="A300" t="s">
         <v>14</v>
       </c>
@@ -17041,7 +17040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:38" hidden="1">
+    <row r="301" spans="1:38">
       <c r="A301" t="s">
         <v>14</v>
       </c>
@@ -17142,7 +17141,7 @@
         <v>5.2749446361410799</v>
       </c>
     </row>
-    <row r="303" spans="1:38" hidden="1">
+    <row r="303" spans="1:38">
       <c r="A303" t="s">
         <v>14</v>
       </c>
@@ -17189,7 +17188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:38" hidden="1">
+    <row r="304" spans="1:38">
       <c r="A304" t="s">
         <v>14</v>
       </c>
@@ -17236,7 +17235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:26" hidden="1">
+    <row r="305" spans="1:26">
       <c r="A305" t="s">
         <v>14</v>
       </c>
@@ -17337,7 +17336,7 @@
         <v>30.747951121142297</v>
       </c>
     </row>
-    <row r="307" spans="1:26" hidden="1">
+    <row r="307" spans="1:26">
       <c r="A307" t="s">
         <v>14</v>
       </c>
@@ -17384,7 +17383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:26" hidden="1">
+    <row r="308" spans="1:26">
       <c r="A308" t="s">
         <v>14</v>
       </c>
@@ -17431,7 +17430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:26" hidden="1">
+    <row r="309" spans="1:26">
       <c r="A309" t="s">
         <v>14</v>
       </c>
@@ -17532,7 +17531,7 @@
         <v>25.765741920483489</v>
       </c>
     </row>
-    <row r="311" spans="1:26" hidden="1">
+    <row r="311" spans="1:26">
       <c r="A311" t="s">
         <v>14</v>
       </c>
@@ -17579,7 +17578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:26" hidden="1">
+    <row r="312" spans="1:26">
       <c r="A312" t="s">
         <v>14</v>
       </c>
@@ -17626,7 +17625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:26" hidden="1">
+    <row r="313" spans="1:26">
       <c r="A313" t="s">
         <v>14</v>
       </c>
@@ -17727,7 +17726,7 @@
         <v>21.196272061510136</v>
       </c>
     </row>
-    <row r="315" spans="1:26" hidden="1">
+    <row r="315" spans="1:26">
       <c r="A315" t="s">
         <v>14</v>
       </c>
@@ -17774,7 +17773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:26" hidden="1">
+    <row r="316" spans="1:26">
       <c r="A316" t="s">
         <v>14</v>
       </c>
@@ -17821,7 +17820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:26" hidden="1">
+    <row r="317" spans="1:26">
       <c r="A317" t="s">
         <v>14</v>
       </c>
@@ -17922,7 +17921,7 @@
         <v>15.757838400771089</v>
       </c>
     </row>
-    <row r="319" spans="1:26" hidden="1">
+    <row r="319" spans="1:26">
       <c r="A319" t="s">
         <v>14</v>
       </c>
@@ -17969,7 +17968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:26" hidden="1">
+    <row r="320" spans="1:26">
       <c r="A320" t="s">
         <v>14</v>
       </c>
@@ -18016,7 +18015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:26" hidden="1">
+    <row r="321" spans="1:26">
       <c r="A321" t="s">
         <v>14</v>
       </c>
@@ -18117,7 +18116,7 @@
         <v>29.401922981328966</v>
       </c>
     </row>
-    <row r="323" spans="1:26" hidden="1">
+    <row r="323" spans="1:26">
       <c r="A323" t="s">
         <v>14</v>
       </c>
@@ -18164,7 +18163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:26" hidden="1">
+    <row r="324" spans="1:26">
       <c r="A324" t="s">
         <v>14</v>
       </c>
@@ -18211,7 +18210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:26" hidden="1">
+    <row r="325" spans="1:26">
       <c r="A325" t="s">
         <v>14</v>
       </c>
@@ -18312,7 +18311,7 @@
         <v>50.899819059836311</v>
       </c>
     </row>
-    <row r="327" spans="1:26" hidden="1">
+    <row r="327" spans="1:26">
       <c r="A327" t="s">
         <v>14</v>
       </c>
@@ -18359,7 +18358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:26" hidden="1">
+    <row r="328" spans="1:26">
       <c r="A328" t="s">
         <v>14</v>
       </c>
@@ -18406,7 +18405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:26" hidden="1">
+    <row r="329" spans="1:26">
       <c r="A329" t="s">
         <v>14</v>
       </c>
@@ -18507,7 +18506,7 @@
         <v>24.558059135821743</v>
       </c>
     </row>
-    <row r="331" spans="1:26" hidden="1">
+    <row r="331" spans="1:26">
       <c r="A331" t="s">
         <v>14</v>
       </c>
@@ -18554,7 +18553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:26" hidden="1">
+    <row r="332" spans="1:26">
       <c r="A332" t="s">
         <v>14</v>
       </c>
@@ -18601,7 +18600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:26" hidden="1">
+    <row r="333" spans="1:26">
       <c r="A333" t="s">
         <v>14</v>
       </c>
@@ -18702,7 +18701,7 @@
         <v>42.470371984124505</v>
       </c>
     </row>
-    <row r="335" spans="1:26" hidden="1">
+    <row r="335" spans="1:26">
       <c r="A335" t="s">
         <v>14</v>
       </c>
@@ -18749,7 +18748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:26" hidden="1">
+    <row r="336" spans="1:26">
       <c r="A336" t="s">
         <v>14</v>
       </c>
@@ -18796,7 +18795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:26" hidden="1">
+    <row r="337" spans="1:26">
       <c r="A337" t="s">
         <v>14</v>
       </c>
@@ -18898,46 +18897,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL338" xr:uid="{D9F824F1-C9CA-4B4A-8D6A-E1D6F0626745}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TOSyear3SowFeb21CvCeleraII"/>
-        <filter val="TOSyear3SowFeb21CvCrystal"/>
-        <filter val="TOSyear3SowFeb21CvJade"/>
-        <filter val="TOSyear3SowFeb21CvOnyx"/>
-        <filter val="TOSyear3SowFeb21CvOpal"/>
-        <filter val="TOSyear3SowJan21CvBerken"/>
-        <filter val="TOSyear3SowJan21CvCeleraII"/>
-        <filter val="TOSyear3SowJan21CvCrystal"/>
-        <filter val="TOSyear3SowJan21CvJade"/>
-        <filter val="TOSyear3SowJan21CvOnyx"/>
-        <filter val="TOSyear3SowJan21CvOpal"/>
-        <filter val="TOSyear3SowNov20CvBerken"/>
-        <filter val="TOSyear3SowNov20CvCeleraII"/>
-        <filter val="TOSyear3SowNov20CvCrystal"/>
-        <filter val="TOSyear3SowNov20CvJade"/>
-        <filter val="TOSyear3SowNov20CvOnyx"/>
-        <filter val="TOSyear3SowNov20CvOpal"/>
-        <filter val="TOSyear3SowOct20CvBerken"/>
-        <filter val="TOSyear3SowOct20CvCeleraII"/>
-        <filter val="TOSyear3SowOct20CvCrystal"/>
-        <filter val="TOSyear3SowOct20CvJade"/>
-        <filter val="TOSyear3SowOct20CvOnyx"/>
-        <filter val="TOSyear3SowOct20CvOpal"/>
-        <filter val="TOSyear3SowSept20CvBerken"/>
-        <filter val="TOSyear3SowSept20CvCeleraII"/>
-        <filter val="TOSyear3SowSept20CvCrystal"/>
-        <filter val="TOSyear3SowSept20CvJade"/>
-        <filter val="TOSyear3SowSept20CvOnyx"/>
-        <filter val="TOSyear3SowSept20CvOpal"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="HarvestRipe"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AL290">
     <sortCondition ref="B2:B290"/>
     <sortCondition ref="C2:C290"/>

</xml_diff>